<commit_message>
Update EtsyData.xlsx and fix bugs in MetaHunt.py
</commit_message>
<xml_diff>
--- a/EtsyData.xlsx
+++ b/EtsyData.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,189 +465,189 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Moss Agate Cluster Wedding Band Bridal Moissanite Ring Promise Anniversary Matching Ring Unique Jewelry Half Eternity Band Gift For Love</t>
+          <t>Riverbed Wave Ring. 18K Gold Vermeil over Sterling Silver &amp; Green Enamel. Adjustable.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>44.70</t>
+          <t>58.33</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1742209424/moss-agate-cluster-wedding-band-bridal?click_key=e26f880e811c5c2afa7492af7f6ed295d6d6f316%3A1742209424&amp;click_sum=d98b5eba&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-1&amp;pro=1&amp;frs=1</t>
+          <t>https://www.etsy.com/listing/1890762377/riverbed-wave-ring-18k-gold-vermeil-over?click_key=f21a040358e9c515e80c29a441fb47e7e88ec238%3A1890762377&amp;click_sum=735f36a1&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-1&amp;sca=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(3,077)</t>
+          <t>(42,538)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/27766378/r/il/78fbaf/6148411473/il_340x270.6148411473_fxmi.jpg</t>
+          <t>https://i.etsystatic.com/6401969/r/il/bae740/6765875526/il_340x270.6765875526_60db.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Marquise moss agate wedding band 14K Rose gold wedding band women Half eternity diamond Matching Unique Bridal Stacking Promise gift for her</t>
+          <t>Peridot earrings green earrings August birthstone jewelry Personalized Dangle Earrings Custom Birthstone Earrings birthday gift for her</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>199.00</t>
+          <t>29.32</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1501639226/marquise-moss-agate-wedding-band-14k?click_key=207a69e066ad03cd16686d36df06e538bc5b54aa%3A1501639226&amp;click_sum=fcd92bd3&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-2&amp;pro=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/90776791/peridot-earrings-green-earrings-august?click_key=30580b4770baca07e477a8f8be3936acaa9cc1f4%3A90776791&amp;click_sum=d032d245&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-2&amp;pro=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(817)</t>
+          <t>(16,278)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/31723428/c/1732/1376/236/503/il/4a797b/5055195514/il_340x270.5055195514_f424.jpg</t>
+          <t>https://i.etsystatic.com/6666729/c/782/621/0/287/il/46a4bc/6061329099/il_340x270.6061329099_an55.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GIGANTIC GIA Certified - 3.50 carat - Round Halo Diamond Engagement Ring - Solid Platinum - Luxury - Custom - wedding - Bph024</t>
+          <t>14K Yellow Gold Floral Ring with Mother of Pearl &amp; 0.96 Ct Green Peridot Gemstone CGL Certified Elegant Jewelry adjustable Made To Order</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37,500.00</t>
+          <t>531.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/111125891/gigantic-gia-certified-350-carat-round?click_key=45ad2e6ebfc146ce84e0058aa276aa91b95e9ccb%3A111125891&amp;click_sum=48882cb3&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-3&amp;pro=1&amp;frs=1</t>
+          <t>https://www.etsy.com/listing/4303764453/14k-yellow-gold-floral-ring-with-mother?click_key=f9a170e81004032c8c27fe38afade16b6c6be726%3A4303764453&amp;click_sum=f2aebccf&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-3&amp;pro=1&amp;frs=1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(740)</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/5708111/r/il/f77bc5/569842630/il_340x270.569842630_5r70.jpg</t>
+          <t>https://i.etsystatic.com/57683402/r/il/79b808/6895208857/il_340x270.6895208857_jzm4.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>14K Solid Yellow Gold Necklace Gold Rope Chain, 14K Gold Rope Chain, 14K Rope Chain, Rope Gold Chain, Diamond-Cut, Men, Woman 3mm 4mm 5mm</t>
+          <t>Emerald Ring, Handmade Women's Ring, Turkish Handmade Ring, Authentic Ring, Ottoman Ring, Ladies Ring, 925k Sterling Silver, Cubic Zircon</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>462.60</t>
+          <t>42.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1835440345/14k-solid-yellow-gold-necklace-gold-rope?click_key=536166fc9fcee75b55ff663a484dbf496580497a%3A1835440345&amp;click_sum=d339be31&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-4&amp;pro=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/977242742/emerald-ring-handmade-womens-ring?click_key=e260881bac8e01ab8d42d615d442bc6a4fe3ad4b%3A977242742&amp;click_sum=8cd08bc3&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-4&amp;pro=1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(25,962)</t>
+          <t>(10,361)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/17394950/r/il/c334f4/6473755552/il_340x270.6473755552_e62n.jpg</t>
+          <t>https://i.etsystatic.com/22806411/c/1342/1067/218/189/il/65d520/3106195309/il_340x270.3106195309_d8y8.jpg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dainty Minimalist Name Necklace, 18K Gold Plated Name Necklace, Personalized Minimalist Name Necklace, Custom Name Jewelry,Mother's Day Gift</t>
+          <t>Coquette Fairycore Themed Mystery Jewelry Jar, Curated Jewelry Jars of Necklaces, Bracelets, Rings &amp; Earrings, Gift for Her</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18.03</t>
+          <t>14.57</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1696930030/dainty-minimalist-name-necklace-18k-gold?click_key=dbadd18327a647caee01d74c52c2aa8e31e6be6d%3A1696930030&amp;click_sum=a026c665&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-1&amp;pro=1&amp;sts=1&amp;content_source=dbadd18327a647caee01d74c52c2aa8e31e6be6d%253A1696930030</t>
+          <t>https://www.etsy.com/listing/4303224938/coquette-fairycore-themed-mystery?click_key=c596ff9e5dfe6fb3914fb4b93d905c99fdc44c99%3A4303224938&amp;click_sum=dcd16ab9&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-1&amp;pro=1&amp;content_source=c596ff9e5dfe6fb3914fb4b93d905c99fdc44c99%253A4303224938</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(41,461)</t>
+          <t>(165)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/34379934/c/1869/1484/109/375/il/2da8e5/5911526940/il_340x270.5911526940_6p5r.jpg</t>
+          <t>https://i.etsystatic.com/55418552/r/il/7e93ad/6871013788/il_340x270.6871013788_s8eq.jpg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Custom Name Necklace, 18K Gold Plated Name Necklace, Personalized Name Necklace, Birthday Gift for Her, Mother's Day Gift, Gift for Mom</t>
+          <t>Mystery Jewelry Jar - Modern Minimalist Theme, Curated Jewelry Jars of Necklaces, Bracelets, Rings &amp; Earrings, Gift for Her</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15.26</t>
+          <t>14.57</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1413455244/custom-name-necklace-18k-gold-plated?click_key=9f8177ccff371f2e14240a261f33bef77fa96bdb%3A1413455244&amp;click_sum=7475517b&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-2&amp;pro=1&amp;sts=1&amp;content_source=9f8177ccff371f2e14240a261f33bef77fa96bdb%253A1413455244</t>
+          <t>https://www.etsy.com/listing/1814825794/mystery-jewelry-jar-modern-minimalist?click_key=d0f9de7ba80eb8de3283154678368daa84bf983b%3A1814825794&amp;click_sum=225a3b4b&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-2&amp;pro=1&amp;content_source=d0f9de7ba80eb8de3283154678368daa84bf983b%253A1814825794</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(41,461)</t>
+          <t>(165)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/34379934/c/2000/1589/0/264/il/628644/4796937795/il_340x270.4796937795_qnr6.jpg</t>
+          <t>https://i.etsystatic.com/55418552/r/il/64296c/6919382099/il_340x270.6919382099_olei.jpg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Personalized Italian Bracelet, Custom Gold Italy Charms, Gold Italian Bracelet, Italy Charms, Gold Italian Charm Bracelet, Gift for Her</t>
+          <t>Mystery Jewelry Jars, Witchy Whimsical Gothic Jewelry Jar, Mystery Jewelry Lot of Necklaces Pendants Bracelets Rings Earrings, Gift for Her</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>24.53</t>
+          <t>14.57</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1798191819/personalized-italian-bracelet-custom?click_key=94508d9c63c8569aebb611947c2ad9bd077646c0%3A1798191819&amp;click_sum=04ae7a6e&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-3&amp;pro=1&amp;sts=1&amp;content_source=94508d9c63c8569aebb611947c2ad9bd077646c0%253A1798191819</t>
+          <t>https://www.etsy.com/listing/4302282840/mystery-jewelry-jars-witchy-whimsical?click_key=7ac3e28109134db857f6fb68eaf4301f0564f7d8%3A4302282840&amp;click_sum=4311c83a&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-3&amp;pro=1&amp;content_source=7ac3e28109134db857f6fb68eaf4301f0564f7d8%253A4302282840</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>(770)</t>
+          <t>(165)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53495552/r/il/59bdad/6338540867/il_340x270.6338540867_htw1.jpg</t>
+          <t>https://i.etsystatic.com/55418552/r/il/94ad99/6893941603/il_340x270.6893941603_4oaj.jpg</t>
         </is>
       </c>
     </row>
@@ -659,498 +659,498 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>31.93</t>
+          <t>33.34</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1848387676/mystery-jewellery-jars?click_key=9e78b37fd937d09722add4092d9c42fe87962a33%3A1848387676&amp;click_sum=79e9ea0a&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-4&amp;bes=1&amp;content_source=9e78b37fd937d09722add4092d9c42fe87962a33%253A1848387676</t>
+          <t>https://www.etsy.com/listing/4304484065/mystery-jewellery-jars?click_key=ec4005a2a8e55fa78cb1a8b7adb57e85aadda601%3A4304484065&amp;click_sum=35278339&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-4&amp;cns=1&amp;content_source=ec4005a2a8e55fa78cb1a8b7adb57e85aadda601%253A4304484065</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(39)</t>
+          <t>(41)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/56707580/r/il/4d8ecc/6635068695/il_340x270.6635068695_lcvh.jpg</t>
+          <t>https://i.etsystatic.com/56707580/r/il/f1a992/6857333856/il_340x270.6857333856_rwfo.jpg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Custom Jewelry,Jewelry Design,Custom Made,Jewelry Making,Personalized Jewelry</t>
+          <t>Vintage Gold Watch Bracelet,Retro Timepiece Jewelry,Elegant Tiger Eye Clock Bracelet,Unique Handmade Fashion Accessory,Luxury Jewelry Gift</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>365.00</t>
+          <t>26.30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1286674540/custom-jewelryjewelry-designcustom?click_key=e3e0964ea4e355da48b03ca509ae1ff9afc528a2%3A1286674540&amp;click_sum=bcabf787&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-5&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=e3e0964ea4e355da48b03ca509ae1ff9afc528a2%253A1286674540</t>
+          <t>https://www.etsy.com/listing/4297824541/vintage-gold-watch-braceletretro?click_key=21bc9e0b51b1208748c851a9222ed917b6f9f75f%3A4297824541&amp;click_sum=50aaf822&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-5&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=21bc9e0b51b1208748c851a9222ed917b6f9f75f%253A4297824541</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(565)</t>
+          <t>(85)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/23761201/r/il/c332b4/4143374776/il_340x270.4143374776_9trm.jpg</t>
+          <t>https://i.etsystatic.com/53454032/r/il/ec1c39/6824047770/il_340x270.6824047770_fjpd.jpg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Baguette Birthstone Necklace, Family Birthstone Necklace, Personalized Gift, Mother's Birthstone Jewelry ,Gift for Mom,Birthday Gift</t>
+          <t>Custom Name Necklace, 18K Gold Plated Name Necklace, Personalized Name Necklace, Birthday Gift for Her, Mother's Day Gift, Gift for Mom</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>29.60</t>
+          <t>15.27</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1806011672/baguette-birthstone-necklace-family?click_key=6fa6ce5ba14528230954477d2178ec3ab18741fc%3A1806011672&amp;click_sum=37c27810&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-6&amp;pro=1&amp;sts=1&amp;content_source=6fa6ce5ba14528230954477d2178ec3ab18741fc%253A1806011672</t>
+          <t>https://www.etsy.com/listing/1413455244/custom-name-necklace-18k-gold-plated?click_key=ab3a07bdc289f3abf4462cdddca5884bab39cf94%3A1413455244&amp;click_sum=ac666f10&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-6&amp;pro=1&amp;sts=1&amp;content_source=ab3a07bdc289f3abf4462cdddca5884bab39cf94%253A1413455244</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>(433)</t>
+          <t>(41,773)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/55594479/c/1298/1298/247/859/il/f1da75/6409042796/il_340x270.6409042796_tb76.jpg</t>
+          <t>https://i.etsystatic.com/34379934/c/2000/1589/0/264/il/628644/4796937795/il_340x270.4796937795_qnr6.jpg</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>14K Gold Name Necklace, Personalized Name Pendant Necklace, Custom Name Necklace, Minimalist Name Jewelry for Women, Gift for Her</t>
+          <t>Custom Italian Charm Bracelet, Gold Italy Charms Bracelet, Vintage Best Friend Bracelet, Handmade Italian Watch Bracelets for Women Gifts</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>16.89</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1574315669/14k-gold-name-necklace-personalized-name?click_key=88cf74df278611bcf8e34c60934ca8c07c4df06e%3A1574315669&amp;click_sum=8be163de&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-7&amp;pro=1&amp;sts=1&amp;content_source=88cf74df278611bcf8e34c60934ca8c07c4df06e%253A1574315669</t>
+          <t>https://www.etsy.com/listing/1873039828/custom-italian-charm-bracelet-gold-italy?click_key=ee4b62be2ea4d8bb174a4fcfdf2b2daf0c8b8986%3A1873039828&amp;click_sum=f4c1a16d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-7&amp;pro=1&amp;sts=1&amp;content_source=ee4b62be2ea4d8bb174a4fcfdf2b2daf0c8b8986%253A1873039828</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>(30,450)</t>
+          <t>(125)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/24042361/r/il/99d870/6390144616/il_340x270.6390144616_33ox.jpg</t>
+          <t>https://i.etsystatic.com/11609255/c/1724/1724/108/115/il/536f9e/6710479364/il_340x270.6710479364_lwo1.jpg</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pink Peach Blossom Open Ring,Ring for women,Fashion jewelry,Gift for her Rose Gold Plating</t>
+          <t>VVS1 Tennis Bracelet, 2-4MM Moissanite &amp; 925 Sterling Silver, Sparkling Moissanite, Passes Diamond Tester</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>20.52</t>
+          <t>67.45</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1805128091/pink-peach-blossom-open-ringring-for?click_key=1cfe9a6659d8df4c16639c15dfb5088bc53782b0%3A1805128091&amp;click_sum=346b6732&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-8&amp;pro=1&amp;frs=1&amp;content_source=1cfe9a6659d8df4c16639c15dfb5088bc53782b0%253A1805128091</t>
+          <t>https://www.etsy.com/listing/1853948798/vvs1-tennis-bracelet-2-4mm-moissanite?click_key=e847394a3bd9a76ceb57e5e55e1684a449e02e12%3A1853948798&amp;click_sum=bc4672b3&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-8&amp;pro=1&amp;frs=1&amp;content_source=e847394a3bd9a76ceb57e5e55e1684a449e02e12%253A1853948798</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(275)</t>
+          <t>(29)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/52310599/r/il/9001c9/6325150620/il_340x270.6325150620_hxsn.jpg</t>
+          <t>https://i.etsystatic.com/56024009/r/il/8e110b/6741930986/il_340x270.6741930986_kerr.jpg</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>If Friends were Flowers I'd Pick You Ring Dish,Personalized Birth Flower Jewelry Dish,Floral Trinket Dish for Friend,Birthday Gift for BFF</t>
+          <t>Natural Rainbow Moonstone 925 Sterling Silver Oval Shape Adjustable Bracelet, Gemstone Jewelry, Tennis Bracelet, Gift For Her, Gift For Love</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8.94</t>
+          <t>14.15</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1813761409/if-friends-were-flowers-id-pick-you-ring?click_key=7d670fb9364cc31d3ac023b4e22f53aa63e34664%3A1813761409&amp;click_sum=1d2849ca&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-9&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=7d670fb9364cc31d3ac023b4e22f53aa63e34664%253A1813761409</t>
+          <t>https://www.etsy.com/listing/1310205516/natural-rainbow-moonstone-925-sterling?click_key=c1618432a06024897693ec3927371e18694090b4%3A1310205516&amp;click_sum=681aa697&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-9&amp;pro=1&amp;content_source=c1618432a06024897693ec3927371e18694090b4%253A1310205516</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>(2,603)</t>
+          <t>(8,748)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/48621519/c/1785/1785/107/81/il/a655af/6417461479/il_340x270.6417461479_pi4e.jpg</t>
+          <t>https://i.etsystatic.com/37557222/r/il/fa25a9/4247357962/il_340x270.4247357962_kv3m.jpg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mystery glass with vintage jewelry</t>
+          <t>Personalized Italian Bracelet, Custom Gold Italy Charms, Gold Italian Bracelet, Italy Charms, Gold Italian Charm Bracelet, Gift for Her</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>43.53</t>
+          <t>24.42</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/4300999122/mystery-glass-with-vintage-jewelry?click_key=fd7ba466502b815738589f24cc413b4d5ceef735%3A4300999122&amp;click_sum=992be42f&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-10&amp;content_source=fd7ba466502b815738589f24cc413b4d5ceef735%253A4300999122</t>
+          <t>https://www.etsy.com/listing/1798191819/personalized-italian-bracelet-custom?click_key=47fe96df04b7e560b8de063c005766be59e9b54b%3A1798191819&amp;click_sum=1d34d9bf&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-10&amp;pro=1&amp;sts=1&amp;content_source=47fe96df04b7e560b8de063c005766be59e9b54b%253A1798191819</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>(8)</t>
+          <t>(829)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/35026475/r/il/02fb78/6888034091/il_340x270.6888034091_nbrl.jpg</t>
+          <t>https://i.etsystatic.com/53495552/r/il/59bdad/6338540867/il_340x270.6338540867_htw1.jpg</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Custom Groomsmen Gifts, Groomsmen Proposal, Gold Plated Initial Cufflinks, Wedding Gift, Cufflinks for Groom, Father, Best Man Proposal</t>
+          <t>Silver Italian Bracelets, 18 Links Italian Bracelets, Vintage Italian Bracelets, Personalized Italian Bracelets</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>9.41</t>
+          <t>15.60</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1725334041/custom-groomsmen-gifts-groomsmen?click_key=1315c34c5187923a96e5666bb929944673556a2e%3A1725334041&amp;click_sum=0261401d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-11&amp;pro=1&amp;frs=1&amp;content_source=1315c34c5187923a96e5666bb929944673556a2e%253A1725334041</t>
+          <t>https://www.etsy.com/listing/1848633141/silver-italian-bracelets-18-links?click_key=2cb6a7e919f0ce6bb5f9f296b0cb86654ce6db39%3A1848633141&amp;click_sum=bc2121cf&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-11&amp;pro=1&amp;content_source=2cb6a7e919f0ce6bb5f9f296b0cb86654ce6db39%253A1848633141</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>(1,932)</t>
+          <t>(344)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/43184250/c/1142/908/249/874/il/87995a/6018882143/il_340x270.6018882143_kahf.jpg</t>
+          <t>https://i.etsystatic.com/53633588/r/il/07335b/6523810440/il_340x270.6523810440_t87i.jpg</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2 Names Necklace with Heart, Personalized Couple Names Necklace, Name Necklace Gift for Mom, Two Name Necklace, Gift for Wife, Mom of Two</t>
+          <t>Blohsh Symbol Dog Tag Necklace｜High Quality Stainless Steel Polished｜Waterproof and Rustproof Design｜Men's and Women's Fashion Accessories</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>20.06</t>
+          <t>10.23</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1777488475/2-names-necklace-with-heart-personalized?click_key=1c80cb9fb8d9ed789af88f70db6859a40f3aff83%3A1777488475&amp;click_sum=aecf3aa2&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-12&amp;pro=1&amp;frs=1&amp;content_source=1c80cb9fb8d9ed789af88f70db6859a40f3aff83%253A1777488475</t>
+          <t>https://www.etsy.com/listing/4298141396/blohsh-symbol-dog-tag-necklacehigh?click_key=2423b555f1811f7dc0d1b776549648d81bf98319%3A4298141396&amp;click_sum=06721012&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-12&amp;pro=1&amp;content_source=2423b555f1811f7dc0d1b776549648d81bf98319%253A4298141396</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>(738)</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53277887/c/2000/2000/0/0/il/37b131/6514071229/il_340x270.6514071229_7dpi.jpg</t>
+          <t>https://i.etsystatic.com/59133224/r/il/c3b910/6825611024/il_340x270.6825611024_brfx.jpg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Green Moss Agate Gemstone Beaded Minimalist Choker, Small Small Beads Beaded Women Necklace, Waterproof Crystal Choker, Healing Jewelry Gift</t>
+          <t>Adorable Kids Birthstone Necklace Personalized Birthday Gift for Little Girls Dainty Birthday Gift Gemstone Charm Necklace for Child</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>43.00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1718060256/green-moss-agate-gemstone-beaded?click_key=e81bddb4244aa507782063399c19e2e4cdfdf56a%3A1718060256&amp;click_sum=685b9f38&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-5&amp;pro=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/1515508065/adorable-kids-birthstone-necklace?click_key=07a5fd7460664c55b63acadfde4a2d370071d37e%3A1515508065&amp;click_sum=3150b01d&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-5&amp;bes=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>(10,717)</t>
+          <t>(21,234)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/40319886/r/il/1dd3a9/5993845192/il_340x270.5993845192_5dka.jpg</t>
+          <t>https://i.etsystatic.com/10230423/r/il/9249dd/5408070742/il_340x270.5408070742_oebv.jpg</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Memorial Leather Bracelet Keepsake for Human and Pet Ashes Mourning Gift, Urn Bracelet</t>
+          <t>0.30 Ct Diamond Stud Earring Round Diamond Solitaire Earrings 14k Yellow Gold 14K White Gold 14K Rose gold</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>77.80</t>
+          <t>29.98</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1770238078/memorial-leather-bracelet-keepsake-for?click_key=08736a8b571e99123279c2a87b551bb1f56e8ead%3A1770238078&amp;click_sum=bd4651aa&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-6&amp;pro=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/551905860/030-ct-diamond-stud-earring-round?click_key=fd710bbb9d2ecc3904a174d82e56b9a97ca1dc61%3A551905860&amp;click_sum=31b74b9e&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-6&amp;bes=1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>(78)</t>
+          <t>(2,381)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/52436607/r/il/2c7890/6745658119/il_340x270.6745658119_nf87.jpg</t>
+          <t>https://i.etsystatic.com/15822554/c/1829/1453/176/246/il/bcee16/1413433427/il_340x270.1413433427_pqgk.jpg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tiger Eye &amp; Black Onyx Natural Stone Adjustable Bracelet, Gift for Him, Best for Husband, Dad, Spiritual Healing Protection Powerful, Men's</t>
+          <t>Travel &amp; Storage Watch Roll For 4 Watches With Stand Function - Watch Box For Storage - Epsom Leather - Men's Gift - Color: BLACK</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>29.99</t>
+          <t>474.28</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1844833272/tiger-eye-black-onyx-natural-stone?click_key=33d19ae94e7052e7772c9794c3c52bd1f2a9c4f8%3A1844833272&amp;click_sum=5d90d511&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-7&amp;pro=1</t>
+          <t>https://www.etsy.com/listing/1060896422/travel-storage-watch-roll-for-4-watches?click_key=1884d1a8a3f3a2ad13f63ddb39566efdc0cccc34%3A1060896422&amp;click_sum=c1fdb05a&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-7&amp;frs=1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>(322)</t>
+          <t>(247)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/51984534/r/il/003845/6617604445/il_340x270.6617604445_jwfx.jpg</t>
+          <t>https://i.etsystatic.com/13579477/r/il/2a77b5/3291321912/il_340x270.3291321912_bsbr.jpg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Star of David Necklace in Yellow Gold • Blue Enamel Magen David Pendant • Israeli Jewish Jewelry • Bar Mitzvah Gift • Western Wall Design</t>
+          <t>Vintage Lab Created Emerald 10K Rose Gold Engagement Ring Art Deco Nature Inspired Leaf Wedding Ring Gift For Women Promise Moissanite Ring</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>585.90</t>
+          <t>116.20</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/4303995659/star-of-david-necklace-in-yellow-gold?click_key=40b9ff9d6e2aef42de7477238c633112b8e8bfd7%3A4303995659&amp;click_sum=5044f41b&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-8&amp;pro=1&amp;frs=1</t>
+          <t>https://www.etsy.com/listing/1621460129/vintage-lab-created-emerald-10k-rose?click_key=1667f73d87c720518f8aa2c949a2ed2cf57af834%3A1621460129&amp;click_sum=7a94d986&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-8&amp;pro=1&amp;frs=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>(120)</t>
+          <t>(348)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/11985312/r/il/471e1a/6902845687/il_340x270.6902845687_erin.jpg</t>
+          <t>https://i.etsystatic.com/43099566/r/il/97dc80/5547706040/il_340x270.5547706040_jcsq.jpg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Silver Italian Bracelets, 18 Links Italian Bracelets, Vintage Italian Bracelets, Personalized Italian Bracelets</t>
+          <t>Pink Peach Blossom Open Ring,Ring for women,Fashion jewelry,Gift for her Rose Gold Plating</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>15.60</t>
+          <t>20.52</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1848633141/silver-italian-bracelets-18-links?click_key=f67af218e9b15542bc9fbb60ec6f9cd389d8741b%3A1848633141&amp;click_sum=caf3378b&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-13&amp;pro=1&amp;content_source=f67af218e9b15542bc9fbb60ec6f9cd389d8741b%253A1848633141</t>
+          <t>https://www.etsy.com/listing/1805128091/pink-peach-blossom-open-ringring-for?click_key=ef0ae277d55930f83823a04fad48d28e5819cf00%3A1805128091&amp;click_sum=088b30cb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-13&amp;pro=1&amp;frs=1&amp;content_source=ef0ae277d55930f83823a04fad48d28e5819cf00%253A1805128091</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>(336)</t>
+          <t>(296)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53633588/r/il/07335b/6523810440/il_340x270.6523810440_t87i.jpg</t>
+          <t>https://i.etsystatic.com/52310599/r/il/9001c9/6325150620/il_340x270.6325150620_hxsn.jpg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Mystery Jewelry Jars, Minimalist &amp; Modern Mystery Jewelry Jar, Mystery Jewelry Lot of Necklaces Pendants Bracelet Ring Earring, Gift for Her</t>
+          <t>Custom Birthflower Necklace with Birthstone, Family Birth Flower Necklacce, Birth Month Necklace, Bridesmaids Gift for Her, Mothers Day Gift</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>13.63</t>
+          <t>13.88</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1814825794/mystery-jewelry-jars-minimalist-modern?click_key=477a6dc89a4e541744d296b2fe8e187d31f0e32d%3A1814825794&amp;click_sum=3af59420&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-14&amp;pro=1&amp;content_source=477a6dc89a4e541744d296b2fe8e187d31f0e32d%253A1814825794</t>
+          <t>https://www.etsy.com/listing/1706218238/custom-birthflower-necklace-with?click_key=9f9b17059aab6d4f61e202a05d9ea6592b74f0f2%3A1706218238&amp;click_sum=a349f296&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-14&amp;pro=1&amp;sts=1&amp;content_source=9f9b17059aab6d4f61e202a05d9ea6592b74f0f2%253A1706218238</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>(139)</t>
+          <t>(1,595)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/55418552/r/il/189bb8/6714142704/il_340x270.6714142704_1t1f.jpg</t>
+          <t>https://i.etsystatic.com/51686135/c/1123/892/476/758/il/b391c7/6018489414/il_340x270.6018489414_5ijh.jpg</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sterling Silver Name Necklace, Dainty Name Necklace, Nameplate Necklace, Custom Gold Jewelry, Personalized Gifts for Her, Mothers Day Gift</t>
+          <t>Pressed Flower Jewelry Set – Real Pansy Pendant and Earrings – Botanical Glass Jewelry – Nature Gift for Her – Violet Flower Jewelry</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16.64</t>
+          <t>57.00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1515524800/sterling-silver-name-necklace-dainty?click_key=1988fc0967d522791288747f57c823425e0802bf%3A1515524800&amp;click_sum=65222ea4&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-15&amp;pro=1&amp;content_source=1988fc0967d522791288747f57c823425e0802bf%253A1515524800</t>
+          <t>https://www.etsy.com/listing/4300565424/pressed-flower-jewelry-set-real-pansy?click_key=a7791f6c56c92c5567ed8b157e416b8d4af8d33c%3A4300565424&amp;click_sum=513905fe&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-15&amp;pro=1&amp;content_source=a7791f6c56c92c5567ed8b157e416b8d4af8d33c%253A4300565424</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>(2,255)</t>
+          <t>(716)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/36792788/c/1666/1324/128/405/il/01febb/5166570685/il_340x270.5166570685_52vo.jpg</t>
+          <t>https://i.etsystatic.com/19164025/r/il/fd87ee/6842562520/il_340x270.6842562520_3nw2.jpg</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>14k Gold Emerald Heart Necklace, Minimalist Heart Shaped Emerald Love Pendant Necklace, Heart Cut Emerald Birthstone Jewelry, Gift for Her</t>
+          <t>14G Dagger Industrial Barbell/Retro textured Industrial Jewelry/Industrial Piercing/Scaffold Jewelry/Industrial Earring/Staight Barbell/Gift</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>30.00</t>
+          <t>10.49</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1775155890/14k-gold-emerald-heart-necklace?click_key=0981f8e77f73fe68c66642fcfc90da03811bc465%3A1775155890&amp;click_sum=5e6fa11a&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-16&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=0981f8e77f73fe68c66642fcfc90da03811bc465%253A1775155890</t>
+          <t>https://www.etsy.com/listing/4304168382/14g-dagger-industrial-barbellretro?click_key=8e00cf02dba45f43d08a71a76a03a478a97b64b1%3A4304168382&amp;click_sum=0d214499&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-16&amp;pro=1&amp;sts=1&amp;content_source=8e00cf02dba45f43d08a71a76a03a478a97b64b1%253A4304168382</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>(100)</t>
+          <t>(88,399)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/51548529/c/1874/1874/495/562/il/dc2972/6249655746/il_340x270.6249655746_9fwx.jpg</t>
+          <t>https://i.etsystatic.com/21623448/c/1834/1834/82/82/il/d05fed/6855794862/il_340x270.6855794862_9mtp.jpg</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Silver Chain Necklace, Curb Chain, Figaro Chain,Paperclip,Box,RopeTwist Chain,Mothers Day Gift, Mother’s Day Gifts,Gift For Her,Gift For Him</t>
+          <t>18K Gold Filled Bracelets,Paperclip Chain,Herringbone Chain,Rope,Snake Chain Bracelet,Everyday Bracelet,Dainty Bracelet,Minimalist Bracelet</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26.37</t>
+          <t>15.99</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1594436172/silver-chain-necklace-curb-chain-figaro?click_key=d5ed223e121d2bb360e7c33f5828521ac61e2797%3A1594436172&amp;click_sum=39dcc3a6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-17&amp;pro=1&amp;frs=1&amp;content_source=d5ed223e121d2bb360e7c33f5828521ac61e2797%253A1594436172</t>
+          <t>https://www.etsy.com/listing/1811798767/18k-gold-filled-braceletspaperclip?click_key=0119f2eaa69e8da6892f4511adb0a4d51d4ed88a%3A1811798767&amp;click_sum=e9932098&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-17&amp;pro=1&amp;sts=1&amp;content_source=0119f2eaa69e8da6892f4511adb0a4d51d4ed88a%253A1811798767</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>(3,230)</t>
+          <t>(2,914)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/37567900/r/il/055010/5494457044/il_340x270.5494457044_81xz.jpg</t>
+          <t>https://i.etsystatic.com/51464338/r/il/6ca537/6407812703/il_340x270.6407812703_7pp9.jpg</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Handmade Crystal Earrings | Natural Amethyst &amp; Quartz | Unique Gemstone Jewelry | Elegant Dangle Earrings | Perfect Gift for Her</t>
+          <t>Heart and Sword Couple Necklace Set - 2pcs Silver Plated Necklaces - Matching His and Hers Jewelry</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2.34</t>
+          <t>19.45</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1775999728/handmade-crystal-earrings-natural?click_key=342916da2cf019151b47b1fdcdfb94220b79cef5%3A1775999728&amp;click_sum=b4df63f1&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-18&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=342916da2cf019151b47b1fdcdfb94220b79cef5%253A1775999728</t>
+          <t>https://www.etsy.com/listing/1836962223/heart-and-sword-couple-necklace-set-2pcs?click_key=d876ba2fb695127ccbdb4bb27889130a9babcf2c%3A1836962223&amp;click_sum=2af1b699&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-18&amp;pro=1&amp;content_source=d876ba2fb695127ccbdb4bb27889130a9babcf2c%253A1836962223</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1160,1033 +1160,2761 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53750222/r/il/fb64a6/6253674540/il_340x270.6253674540_bbt2.jpg</t>
+          <t>https://i.etsystatic.com/49738791/r/il/9622fe/6528189735/il_340x270.6528189735_ak2j.jpg</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Iced Out Personalized Big Name Pendant with 12mm Cuban Link Chain,Custom Name Necklace,Custom Chain,Hiphop Jewelry,Custom Birthday Gifts</t>
+          <t>Green Copper Turquoise Bangle, 925 Silver Bangle, Handmade Bangle, Women Bangle, Adjustable Bangle, Everyday Bangle, Silver Bracelet Jewelry</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>27.60</t>
+          <t>18.01</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1683162610/iced-out-personalized-big-name-pendant?click_key=536bf3e6b1ddf60ea26499bf11bc131d520f3018%3A1683162610&amp;click_sum=7f6cf3fa&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-19&amp;pro=1&amp;sts=1&amp;content_source=536bf3e6b1ddf60ea26499bf11bc131d520f3018%253A1683162610</t>
+          <t>https://www.etsy.com/listing/1365985292/green-copper-turquoise-bangle-925-silver?click_key=9df7e5605dc2d371ae376ac2d67e05ef50d2b689%3A1365985292&amp;click_sum=8e472563&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-19&amp;pro=1&amp;content_source=9df7e5605dc2d371ae376ac2d67e05ef50d2b689%253A1365985292</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>(2,398)</t>
+          <t>(8,748)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/25298655/c/2992/2376/0/76/il/85a58a/5901019163/il_340x270.5901019163_3cuh.jpg</t>
+          <t>https://i.etsystatic.com/37557222/r/il/d8a2eb/4463869778/il_340x270.4463869778_2sv9.jpg</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18K Gold Filled Chain Necklace,Curb,Figaro,Rope,Paperclip Chain,Herringbone Chain,twist Chain,Gift For Her,Gift for him, Mother’s Day Gifts</t>
+          <t>2 Names Necklace with Heart, Personalized Couple Names Necklace, Name Necklace Gift for Mom, Two Name Necklace, Gift for Wife, Mom of Two</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>22.07</t>
+          <t>20.08</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1624025579/18k-gold-filled-chain?click_key=a390500e70b0c3cb24528e7aa2b9d74d068fa6c9%3A1624025579&amp;click_sum=9ecbfd80&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-20&amp;pro=1&amp;frs=1&amp;content_source=a390500e70b0c3cb24528e7aa2b9d74d068fa6c9%253A1624025579</t>
+          <t>https://www.etsy.com/listing/1777488475/2-names-necklace-with-heart-personalized?click_key=64820679e7a5f2bfc925e9ac9e68bd5f7c8af710%3A1777488475&amp;click_sum=ca38b20d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-20&amp;pro=1&amp;frs=1&amp;content_source=64820679e7a5f2bfc925e9ac9e68bd5f7c8af710%253A1777488475</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>(3,230)</t>
+          <t>(770)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/37567900/r/il/901062/5557563622/il_340x270.5557563622_4gjd.jpg</t>
+          <t>https://i.etsystatic.com/53277887/c/2000/2000/0/0/il/37b131/6514071229/il_340x270.6514071229_7dpi.jpg</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Personalized Arabic Name Necklace, Custom 18K Gold Name Necklace, Arabic Calligraphy Name Necklace, Islamic Gift, Eid Gift,Mother's Day Gift</t>
+          <t>Italian Bracelet,Custom silver Italy Charms,Personalized Italian Bracelet,Evil Eye Charms,Jewelry Gifts for Her,Birthday gift,Christmas gift</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>23.58</t>
+          <t>21.09</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1234664395/personalized-arabic-name-necklace-custom?click_key=caba298e21b58c0a7735f497cf0810d6a9c24731%3A1234664395&amp;click_sum=b91a772c&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-21&amp;pro=1&amp;sts=1&amp;content_source=caba298e21b58c0a7735f497cf0810d6a9c24731%253A1234664395</t>
+          <t>https://www.etsy.com/listing/1787047600/italian-braceletcustom-silver-italy?click_key=96fd252e30f5f0098e867d913491535bbbb66ecf%3A1787047600&amp;click_sum=a0f7cc24&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-21&amp;pro=1&amp;sts=1&amp;content_source=96fd252e30f5f0098e867d913491535bbbb66ecf%253A1787047600</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>(41,461)</t>
+          <t>(777)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/34379934/c/1600/1271/252/334/il/3eff41/5668627399/il_340x270.5668627399_dk67.jpg</t>
+          <t>https://i.etsystatic.com/52861665/r/il/63a3fd/6353940707/il_340x270.6353940707_eqs7.jpg</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18K Gold Filled Chain Necklace,Pearl Chain,Curb Chian,Box Chain,Paperclip Chain,Twist Chain,Dainty Chain,Gift for Her,Mothers Day Gifts</t>
+          <t>Iced Out Personalized Big Name Pendant with 12mm Cuban Link Chain,Custom Name Necklace,Custom Chain,Hiphop Jewelry,Custom Birthday Gifts</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11.99</t>
+          <t>27.60</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1782276981/18k-gold-filled-chain-necklacepearl?click_key=2c5f1a3a3f4be147e57c42febe5a188c10968db1%3A1782276981&amp;click_sum=667a6d28&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-22&amp;pro=1&amp;sts=1&amp;content_source=2c5f1a3a3f4be147e57c42febe5a188c10968db1%253A1782276981</t>
+          <t>https://www.etsy.com/listing/1683162610/iced-out-personalized-big-name-pendant?click_key=84df93e7f3b3d723ad2ecd87891c045302cb529f%3A1683162610&amp;click_sum=ba913d06&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-22&amp;pro=1&amp;sts=1&amp;content_source=84df93e7f3b3d723ad2ecd87891c045302cb529f%253A1683162610</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>(2,828)</t>
+          <t>(2,420)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/51464338/r/il/ee68f9/6294619536/il_340x270.6294619536_69q2.jpg</t>
+          <t>https://i.etsystatic.com/25298655/c/2992/2376/0/76/il/85a58a/5901019163/il_340x270.5901019163_3cuh.jpg</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>18K Gold Love Knot Bracelet, Infinity Bracelet, Bridesmaid Gift, Couples Bracelet, Birthday Gift for Her, Mothers Day Gift, Friendship Gift</t>
+          <t>18K Gold Filled Chain Necklace,Curb,Figaro,Rope,Paperclip Chain,Herringbone Chain,twist Chain,Gift For Her,Gift for him, Mother’s Day Gifts</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>13.84</t>
+          <t>22.09</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1790801622/18k-gold-love-knot-bracelet-infinity?click_key=32b32f8976c1dab3eeb52aca9663007b19d408a3%3A1790801622&amp;click_sum=1b839b25&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-23&amp;pro=1&amp;frs=1&amp;content_source=32b32f8976c1dab3eeb52aca9663007b19d408a3%253A1790801622</t>
+          <t>https://www.etsy.com/listing/1624025579/18k-gold-filled-chain?click_key=0a6b0599c20b3a92ce1e7e5fd0cacb12e3619110%3A1624025579&amp;click_sum=25a30898&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-23&amp;pro=1&amp;frs=1&amp;content_source=0a6b0599c20b3a92ce1e7e5fd0cacb12e3619110%253A1624025579</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>(80)</t>
+          <t>(3,268)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53324696/r/il/bfca1a/6810596174/il_340x270.6810596174_5va6.jpg</t>
+          <t>https://i.etsystatic.com/37567900/r/il/901062/5557563622/il_340x270.5557563622_4gjd.jpg</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Custom Italian Charm Bracelet, Gold Italy Charms Bracelet, Vintage Best Friend Bracelet, Handmade Italian Watch Bracelets for Women Gifts</t>
+          <t>Cloisonne Bracelets, Vintage Green/Red/Purple/Blue/Pink/Yellow Enamel Flowers Bracelets, Anniversary Gift, Birthday Gift, Gift for Her</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>17.52</t>
+          <t>12.68</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1873039828/custom-italian-charm-bracelet-gold-italy?click_key=306485d3ef6aa7527a2d67313af43112f994886b%3A1873039828&amp;click_sum=779937c7&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-24&amp;pro=1&amp;sts=1&amp;content_source=306485d3ef6aa7527a2d67313af43112f994886b%253A1873039828</t>
+          <t>https://www.etsy.com/listing/1883423978/cloisonne-bracelets-vintage?click_key=4f48fb370df219942befb090140203572dea029c%3A1883423978&amp;click_sum=9cd4394c&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-24&amp;pro=1&amp;frs=1&amp;content_source=4f48fb370df219942befb090140203572dea029c%253A1883423978</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>(101)</t>
+          <t>(6)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/11609255/c/1724/1724/108/115/il/536f9e/6710479364/il_340x270.6710479364_lwo1.jpg</t>
+          <t>https://i.etsystatic.com/54138066/r/il/ddef71/6812004839/il_340x270.6812004839_mxzm.jpg</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Labradorite Necklace Gold Filled Chain, Layered Necklace Set, Raw Labradorite Stone Necklace, Teardrop Gray Crystal Necklace Gold</t>
+          <t>Mens Bracelet with Stainless Steel Rings • Adjustable Bracelet Men • Waterproof Bracelet Women • Mens Jewelry • Gift For Him</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>36.00</t>
+          <t>16.35</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/782078764/labradorite-necklace-gold-filled-chain?click_key=5ec3ff279b79da20f2e627f899f3cdb351820112%3A782078764&amp;click_sum=d11c321c&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-9&amp;etp=1</t>
+          <t>https://www.etsy.com/listing/1704505485/mens-bracelet-with-stainless-steel-rings?click_key=2e102bc59b01445f4168bb8c51e573978cf12f5e%3A1704505485&amp;click_sum=284fa48f&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-9&amp;etp=1</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>(4,447)</t>
+          <t>(32,683)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/17842620/c/1064/846/473/81/il/765c80/5424707866/il_340x270.5424707866_ikjb.jpg</t>
+          <t>https://i.etsystatic.com/13238741/c/2419/1923/268/454/il/67d10e/5877699290/il_340x270.5877699290_kibf.jpg</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Dainty Flower Pearl Earrings, Floral and Pearl Drop Earrings, Bridal Dangle Earrings, Wedding Earrings, Bridesmaid Gifts for Her, Mom Gifts</t>
+          <t>14K Gold Diamond Cross Necklace for Women | Minimalist Diamond Cross Pendant | 14K Gold Jewelry | Perfect Graduation Gift</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>26.00</t>
+          <t>184.00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1900507375/dainty-flower-pearl-earrings-floral-and?click_key=027e8ef66d84f19fbdde90b07d234ed3cd0fcc45%3A1900507375&amp;click_sum=c8b073ef&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-10&amp;pro=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/1806364223/14k-gold-diamond-cross-necklace-for?click_key=4ecf77b61a7bea8b444e77506a6d63c5f49f06e7%3A1806364223&amp;click_sum=bb19e7fe&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-10&amp;pro=1&amp;frs=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>(223)</t>
+          <t>(19)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/54157745/c/1000/1000/598/579/il/fb98f2/6826819913/il_340x270.6826819913_pp21.jpg</t>
+          <t>https://i.etsystatic.com/54432389/c/1388/1388/400/620/il/a9c600/6331474802/il_340x270.6331474802_om5t.jpg</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14k Real Solid Gold Bismarck Chain Necklace,Ladies Fancy Bismark Link Chain 3.5mm 16,18,20 inches</t>
+          <t>Carnelian Necklace, Gold Carnelian Pendant, Personalized Necklace Gift, Witchy Jewelry, Best Friend Gift, Unique Gift for Her</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>339.00</t>
+          <t>54.24</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1479538052/14k-real-solid-gold-bismarck-chain?click_key=9a7f5a1f21c9974659f5ae18d051b421af019915%3A1479538052&amp;click_sum=f3a71c7f&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-11&amp;pro=1&amp;frs=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/4307066524/carnelian-necklace-gold-carnelian?click_key=1fd4326796facd9376546de8d2e30e61f531dadf%3A4307066524&amp;click_sum=bae7dbe9&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-11</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>(473)</t>
+          <t>(4,458)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/31566437/r/il/69cbd7/5596611926/il_340x270.5596611926_ab3o.jpg</t>
+          <t>https://i.etsystatic.com/17842620/c/1301/1301/143/12/il/19c615/6870317496/il_340x270.6870317496_360x.jpg</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>18K Gold Filled CZ Flower Earrings,Huggie Hoop Earrings,Hoop Earrings,Hypoallergenic Huggie Hoop,Gift for Her</t>
+          <t>14k Gold Dome Wedding Band / Yellow, Rose and White Gold Dome Ring / Matching Wedding Band for Women / Solid Gold Band Ring Sets</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5.74</t>
+          <t>159.75</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1702754778/18k-gold-filled-cz-flower-earringshuggie?click_key=63edf378258be7601ec7916ef9aefe53a662e4cd%3A1702754778&amp;click_sum=d937db98&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-12&amp;pro=1&amp;sts=1</t>
+          <t>https://www.etsy.com/listing/1251774176/14k-gold-dome-wedding-band-yellow-rose?click_key=7e07434aef0d9dd9149e6818122dcdccac6e034f%3A1251774176&amp;click_sum=6bdee5c4&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-12&amp;pro=1&amp;frs=1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>(914)</t>
+          <t>(2,152)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/24923276/c/1562/1241/200/320/il/e7a1f7/5927767518/il_340x270.5927767518_mt60.jpg</t>
+          <t>https://i.etsystatic.com/36471853/c/1804/1434/778/478/il/f3d666/4036768632/il_340x270.4036768632_67hz.jpg</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CH In Box 925 Silver Cross Dice Bullet Dagger Necklace gothic style Y2K rosary Jewelry Birthday Gift 60CM</t>
+          <t>18K Gold Filled Chain Necklace,Pearl Chain,Curb Chian,Box Chain,Paperclip Chain,Twist Chain,Dainty Chain,Gift for Her,Mothers Day Gifts</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>27.79</t>
+          <t>11.99</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1879133636/ch-in-box-925-silver-cross-dice-bullet?click_key=1b26f790260a2a1d6929d5f05d2722e1f63762cb%3A1879133636&amp;click_sum=1889405d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-25&amp;pro=1&amp;sts=1&amp;content_source=1b26f790260a2a1d6929d5f05d2722e1f63762cb%253A1879133636</t>
+          <t>https://www.etsy.com/listing/1782276981/18k-gold-filled-chain-necklacepearl?click_key=7512c3a0ed8136f6a36032c9d8afe6a80d394561%3A1782276981&amp;click_sum=e86065e6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-25&amp;pro=1&amp;sts=1&amp;content_source=7512c3a0ed8136f6a36032c9d8afe6a80d394561%253A1782276981</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>(445)</t>
+          <t>(2,914)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/56470180/r/il/27cca5/6790367919/il_340x270.6790367919_lm3m.jpg</t>
+          <t>https://i.etsystatic.com/51464338/r/il/ee68f9/6294619536/il_340x270.6294619536_69q2.jpg</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Handmade Birthstone Name Necklace, Personalized Name Necklace, Necklace with Birthstone, Christmas Gift for Her, Women Gift for Wedding</t>
+          <t>Labradorite Copper Pendant Copper Wire Wrapped Gemstone Pendant Handmade Copper Wire Jewelry Gift For Wife Labradorite Jewelry Wedding Gift</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>17.07</t>
+          <t>17.06</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1773370947/handmade-birthstone-name-necklace?click_key=77df6f17152556df098b74bacbbae71efa125b3f%3A1773370947&amp;click_sum=47c19047&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-26&amp;pro=1&amp;frs=1&amp;content_source=77df6f17152556df098b74bacbbae71efa125b3f%253A1773370947</t>
+          <t>https://www.etsy.com/listing/1250123390/labradorite-copper-pendant-copper-wire?click_key=78da3d7a6fea1bcd9745c6a64cdb4c750aeaa464%3A1250123390&amp;click_sum=67f43c92&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-26&amp;pro=1&amp;frs=1&amp;content_source=78da3d7a6fea1bcd9745c6a64cdb4c750aeaa464%253A1250123390</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>(738)</t>
+          <t>(15,753)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53277887/c/1587/1587/292/377/il/7142df/6463600074/il_340x270.6463600074_2mu1.jpg</t>
+          <t>https://i.etsystatic.com/10932069/r/il/f8d6d1/4042142991/il_340x270.4042142991_m6hb.jpg</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Family Charm Necklace, Custom Birthstone Initial Necklace, Unique Gift for New Mom, Personalized mom necklace with kids initials Stamped</t>
+          <t>18K Gold Chain Necklace/Cable Chain/Paperclip Chain/Twist Chain/Figaro/Curb Chain/Bead Chain/Blade Chain/Chain for kids/Mothers Day Gifts</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>32.50</t>
+          <t>11.87</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/489997879/family-charm-necklace-custom-birthstone?click_key=9d36dbd51251623f80afb71a695bb25906fa8bff%3A489997879&amp;click_sum=21627792&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-27&amp;pro=1&amp;sts=1&amp;content_source=9d36dbd51251623f80afb71a695bb25906fa8bff%253A489997879</t>
+          <t>https://www.etsy.com/listing/1802574426/18k-gold-chain-necklacecable?click_key=2b2c914da695b8a38776aaa664d23e33c8244e52%3A1802574426&amp;click_sum=d3a4ddd3&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-27&amp;pro=1&amp;frs=1&amp;content_source=2b2c914da695b8a38776aaa664d23e33c8244e52%253A1802574426</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>(87,012)</t>
+          <t>(62)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/6120089/c/1142/908/53/136/il/768e77/4972805688/il_340x270.4972805688_9k6v.jpg</t>
+          <t>https://i.etsystatic.com/54758409/r/il/185c7e/6432383117/il_340x270.6432383117_icqr.jpg</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Letter Necklace,Heart Letter Necklace , Custom Initial Necklace , Gold Custom Gift ,Valentine's Day Gift</t>
+          <t>925 Sterling Silver Rope Chain Necklace,Real Silver Chain,Silver Jewelry Chain Necklaces For Women And Mens ,Choker Chain, Chain for Pendant</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>29.13</t>
+          <t>22.22</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1112000072/letter-necklaceheart-letter-necklace?click_key=8a5b00d916d02f26f611b6a3495760ec7f92ecb9%3A1112000072&amp;click_sum=6fffb9c0&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-28&amp;pro=1&amp;content_source=8a5b00d916d02f26f611b6a3495760ec7f92ecb9%253A1112000072</t>
+          <t>https://www.etsy.com/listing/1740374254/925-sterling-silver-rope-chain?click_key=5339bb59ced00dcda2f37f5cc3c90d30e7449b71%3A1740374254&amp;click_sum=3f3ab6fb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-28&amp;pro=1&amp;frs=1&amp;content_source=5339bb59ced00dcda2f37f5cc3c90d30e7449b71%253A1740374254</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>(5,019)</t>
+          <t>(500)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/24904244/c/612/612/340/524/il/6d5610/6845964201/il_340x270.6845964201_2jy5.jpg</t>
+          <t>https://i.etsystatic.com/52961888/r/il/04f3f3/6188504811/il_340x270.6188504811_56bw.jpg</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Leaf Clover, Clover Model Bracelet 3 Set Gold, White, Black Color Enamel Clover Bracelet 316L Steel Necklace, Green Clover Bracelet</t>
+          <t>Upper arm cuff arm band spiral handmade made of brass, jewelry</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>79.03</t>
+          <t>18.30</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/4296078717/leaf-clover-clover-model-bracelet-3-set?click_key=93d9ea62f375a6733fc23e579220d9a9adcd3e55%3A4296078717&amp;click_sum=cbc08694&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-29&amp;frs=1&amp;content_source=93d9ea62f375a6733fc23e579220d9a9adcd3e55%253A4296078717</t>
+          <t>https://www.etsy.com/listing/1696016225/upper-arm-cuff-arm-band-spiral-handmade?click_key=546f623ddfc4d0e1ff215cb1b0115ef18d3298f0%3A1696016225&amp;click_sum=c0213bf6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-29&amp;pro=1&amp;content_source=546f623ddfc4d0e1ff215cb1b0115ef18d3298f0%253A1696016225</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>(9)</t>
+          <t>(465)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/51174210/r/il/81736d/6815082378/il_340x270.6815082378_fncs.jpg</t>
+          <t>https://i.etsystatic.com/39191393/r/il/218f84/5840542934/il_340x270.5840542934_1llm.jpg</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PERIMADE Silver Bubble Projection Necklace • Customized Memorial Photo Pendant • Personalized Picture Inside Jewelry • Trendy Friend Gift</t>
+          <t>Arcane Pendant &amp; Keychain | Dual-Sided Blue Rose Design | VI, Jinx, Ekko Inspired | Perfect Gift for Fans, League of Legends Hextech cosplay</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16.95</t>
+          <t>21.67</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1238175661/perimade-silver-bubble-projection?click_key=9028d91ac23ee100f82e3a8f9afb218f8ceb6dd8%3A1238175661&amp;click_sum=43961c05&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-30&amp;frs=1&amp;etp=1&amp;sts=1&amp;content_source=9028d91ac23ee100f82e3a8f9afb218f8ceb6dd8%253A1238175661</t>
+          <t>https://www.etsy.com/listing/4298325681/arcane-pendant-keychain-dual-sided-blue?click_key=6eb3f36d71f8f4073da7425bd4e52e79f97811f7%3A4298325681&amp;click_sum=4b217f4a&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-30&amp;pro=1&amp;frs=1&amp;content_source=6eb3f36d71f8f4073da7425bd4e52e79f97811f7%253A4298325681</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>(47,211)</t>
+          <t>(55)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/17618956/r/il/809a76/5401368313/il_340x270.5401368313_gf4g.jpg</t>
+          <t>https://i.etsystatic.com/56411742/r/il/269ede/6874531515/il_340x270.6874531515_pkws.jpg</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Natural Pearl Flower Dangle Earrings, Dainty Pearl Earrings, Drop Pearl Earrings, Wedding Earrings, Bridesmaid Gift, Birthday Gifts for Her</t>
+          <t>Ivan Cornejo, Ivan Cornejo Inspired, Ivan C Inspired Handmade Bracelets</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23.57</t>
+          <t>8.00</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1813144445/natural-pearl-flower-dangle-earrings?click_key=caa5aec0ff11d6a1fdd3e62dfeeb07e77a9233de%3A1813144445&amp;click_sum=42751205&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-31&amp;pro=1&amp;sts=1&amp;content_source=caa5aec0ff11d6a1fdd3e62dfeeb07e77a9233de%253A1813144445</t>
+          <t>https://www.etsy.com/listing/1861748200/ivan-cornejo-ivan-cornejo-inspired-ivan?click_key=24436b4f1e2add9f51988838159d9c75a3824667%3A1861748200&amp;click_sum=33fde49e&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-31&amp;content_source=24436b4f1e2add9f51988838159d9c75a3824667%253A1861748200</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>(639)</t>
+          <t>(964)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53736912/c/1063/1063/432/522/il/084411/6414468897/il_340x270.6414468897_ord9.jpg</t>
+          <t>https://i.etsystatic.com/30749325/r/il/ed4ec4/6652934310/il_340x270.6652934310_c51g.jpg</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>925 Sterling Silver Rope Chain Necklace,Real Silver Chain,Silver Jewelry Chain Necklaces For Women And Mens ,Choker Chain, Chain for Pendant</t>
+          <t>14k Gold Emerald Heart Necklace, Minimalist Heart Shaped Emerald Love Pendant Necklace, Heart Cut Emerald Birthstone Jewelry, Gift for Her</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>22.22</t>
+          <t>30.00</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1740374254/925-sterling-silver-rope-chain?click_key=3a1ff05cd9f9737d7dba0669f450528e927656d4%3A1740374254&amp;click_sum=3c7536fa&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-32&amp;pro=1&amp;frs=1&amp;content_source=3a1ff05cd9f9737d7dba0669f450528e927656d4%253A1740374254</t>
+          <t>https://www.etsy.com/listing/1775155890/14k-gold-emerald-heart-necklace?click_key=8bfe5ee55c1b2883f76d7d1c9db139f3b416b9b7%3A1775155890&amp;click_sum=31d56f15&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-32&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=8bfe5ee55c1b2883f76d7d1c9db139f3b416b9b7%253A1775155890</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>(480)</t>
+          <t>(114)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/52961888/r/il/04f3f3/6188504811/il_340x270.6188504811_56bw.jpg</t>
+          <t>https://i.etsystatic.com/51548529/c/1874/1874/495/562/il/dc2972/6249655746/il_340x270.6249655746_9fwx.jpg</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>14K Solid Gold Family Birthstone Necklace, Personalized Birthstone Necklace, Custom Gift for Mom, Mother's Day Necklace, Gift for Her,</t>
+          <t>handmade dew necklace "wave drops"</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>30.40</t>
+          <t>56.65</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1827149777/14k-solid-gold-family-birthstone?click_key=c195518bdeb1e06e8a4c3558c368c9cc51faf229%3A1827149777&amp;click_sum=8a98f2d4&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-33&amp;pro=1&amp;sts=1&amp;content_source=c195518bdeb1e06e8a4c3558c368c9cc51faf229%253A1827149777</t>
+          <t>https://www.etsy.com/listing/1809936026/handmade-dew-necklace-wave-drops?click_key=25ffd30b6bc9abe2f01e1e5a28d9feef9ce80e09%3A1809936026&amp;click_sum=8938e008&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-33&amp;bes=1&amp;sts=1&amp;content_source=25ffd30b6bc9abe2f01e1e5a28d9feef9ce80e09%253A1809936026</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>(161)</t>
+          <t>(140)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/56014557/r/il/698400/6435496120/il_340x270.6435496120_syse.jpg</t>
+          <t>https://i.etsystatic.com/55955607/r/il/adf9ee/6468934587/il_340x270.6468934587_tbuk.jpg</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Italian Bracelet,Custom silver Italy Charms,Personalized Italian Bracelet,Evil Eye Charms,Jewelry Gifts for Her,Birthday gift,Christmas gift</t>
+          <t>18K Gold Filled Chain Necklace, Curb ,Figaro, Dainty, Rope Chain, Valentines Day,Paperclip Chain,Snake Chain,Mothers Day Gift, Gift For Her</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>21.07</t>
+          <t>23.06</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1787047600/italian-braceletcustom-silver-italy?click_key=5a4e3f82e2950b08ccbfba9f9b06006727ee89b9%3A1787047600&amp;click_sum=50b8c770&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-34&amp;pro=1&amp;sts=1&amp;content_source=5a4e3f82e2950b08ccbfba9f9b06006727ee89b9%253A1787047600</t>
+          <t>https://www.etsy.com/listing/1570883974/18k-gold-filled-chain-necklace-curb?click_key=dced132d0e7e18c824bc21f0bb282501ff2edfa6%3A1570883974&amp;click_sum=8f886f09&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-34&amp;pro=1&amp;frs=1&amp;content_source=dced132d0e7e18c824bc21f0bb282501ff2edfa6%253A1570883974</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>(763)</t>
+          <t>(948)</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/52861665/r/il/63a3fd/6353940707/il_340x270.6353940707_eqs7.jpg</t>
+          <t>https://i.etsystatic.com/47300955/r/il/fe0595/5436560409/il_340x270.5436560409_kvws.jpg</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Personalized Photo Beaded Bracelet, Custom Photo Bracelet, Beaded Projection Photo Bracelet, Anniversary Birthday Gift, Couples Bracelet</t>
+          <t>8mm Adjustable Bangle Bracelet, Colorful Bangle Bracelet, Flower Pattern Enamel Bangle, Women's Bangle Bracelet, Floral Bangles</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18.95</t>
+          <t>15.32</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1533332618/personalized-photo-beaded-bracelet?click_key=ba0775b4785337bd916048eacdc6eb73786ee662%3A1533332618&amp;click_sum=b1010978&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-35&amp;pro=1&amp;frs=1&amp;content_source=ba0775b4785337bd916048eacdc6eb73786ee662%253A1533332618</t>
+          <t>https://www.etsy.com/listing/1876267248/8mm-adjustable-bangle-bracelet-colorful?click_key=649f93ab479f677111d2b79a96d26d1aaab6bead%3A1876267248&amp;click_sum=4d9467de&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-35&amp;pro=1&amp;frs=1&amp;content_source=649f93ab479f677111d2b79a96d26d1aaab6bead%253A1876267248</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>(1,597)</t>
+          <t>(21)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/35109771/c/909/722/73/178/il/4e1a72/5417461757/il_340x270.5417461757_ewwy.jpg</t>
+          <t>https://i.etsystatic.com/57066309/r/il/c5e275/6818479806/il_340x270.6818479806_lq4l.jpg</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18K Gold Filled Chain Necklace, Curb ,Figaro, Dainty, Rope Chain, Valentines Day,Paperclip Chain,Snake Chain,Mothers Day Gift, Gift For Her</t>
+          <t>Handmade Birthstone Name Necklace, Personalized Name Necklace, Necklace with Birthstone, Christmas Gift for Her, Women Gift for Wedding</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>23.04</t>
+          <t>17.09</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1570883974/18k-gold-filled-chain-necklace-curb?click_key=72a415971ab0a4f64055c52cf6abd9a2b50f2691%3A1570883974&amp;click_sum=eec41f7e&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-36&amp;pro=1&amp;frs=1&amp;content_source=72a415971ab0a4f64055c52cf6abd9a2b50f2691%253A1570883974</t>
+          <t>https://www.etsy.com/listing/1773370947/handmade-birthstone-name-necklace?click_key=1fc82e51759cd729859b13944268283526c45c7f%3A1773370947&amp;click_sum=62cbb530&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-36&amp;pro=1&amp;frs=1&amp;content_source=1fc82e51759cd729859b13944268283526c45c7f%253A1773370947</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>(938)</t>
+          <t>(770)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/47300955/r/il/fe0595/5436560409/il_340x270.5436560409_kvws.jpg</t>
+          <t>https://i.etsystatic.com/53277887/c/1587/1587/292/377/il/7142df/6463600074/il_340x270.6463600074_2mu1.jpg</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>14K Gold Tiny Lesbian Jewelry, Scissors Necklace | Minimalist Pride Jewelry | WLW Scissor Bisexual Transgender Necklace | Matching Necklace</t>
+          <t>Elegant Galaxy Healing Oval Blue Sandstone Engagement Ring Moss Agate Wedding Ring Vintage 14k Rose Gold June Birthstone Alexandrite Ring</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>19.19</t>
+          <t>39.90</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1666073983/14k-gold-tiny-lesbian-jewelry-scissors?click_key=4c1701f8b16ea6278e69a3eb84d0252ba38cbdae%3A1666073983&amp;click_sum=707506e5&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-13&amp;pro=1</t>
+          <t>https://www.etsy.com/listing/1779023082/elegant-galaxy-healing-oval-blue?click_key=6f2407c618c62e49da8d680b5c0ad9c5d7ad0aa1%3A1779023082&amp;click_sum=4a1c517c&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-13&amp;pro=1&amp;frs=1</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>(43,707)</t>
+          <t>(664)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/19319642/c/1879/1493/433/345/il/eccc8e/5710762494/il_340x270.5710762494_eynz.jpg</t>
+          <t>https://i.etsystatic.com/42136421/c/1388/1388/305/291/il/ccfaee/6316171943/il_340x270.6316171943_6sly.jpg</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Full Moon Diamond Stud Earrings – Custom Made in 14K or 18K Gold – Italian Celestial Jewelry by Oltremare Gioielli</t>
+          <t>14k Gold Map of Israel pendant, Gold Israel Pendant, Eilat Stone Pendant, Gold Jewish Pendant, Map necklace pendant, Israel Jewelry</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1,790.47</t>
+          <t>693.00</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/4303999729/full-moon-diamond-stud-earrings-custom?click_key=08a0d75e81496d2ae377ad28241b72a94de99c18%3A4303999729&amp;click_sum=c66ca9e1&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-14&amp;pro=1</t>
+          <t>https://www.etsy.com/listing/1555786865/14k-gold-map-of-israel-pendant-gold?click_key=57134af2674895f93ad02c23d338ebe1876a04c3%3A1555786865&amp;click_sum=ca54dd83&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-14&amp;frs=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>(262)</t>
+          <t>(301)</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/18395709/r/il/a3b9a6/6854891986/il_340x270.6854891986_mufc.jpg</t>
+          <t>https://i.etsystatic.com/23295999/r/il/e9cd0b/5300031785/il_340x270.5300031785_9ixt.jpg</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Cross Pendant Necklace , Rosary Cross Necklaces , Dainty Diamond Necklace , Minimalist Religious Necklace , Cross Jewelry , Gift For Her,Mom</t>
+          <t>Vintage kite cut green moss agate engagement ring set 14k rose gold marquise cut diamond ring women unique bridal wedding ring set gift</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>25.89</t>
+          <t>131.20</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1820562079/cross-pendant-necklace-rosary-cross?click_key=76f252b4ba37910776f02dd6c452ae1cf7c2a0a4%3A1820562079&amp;click_sum=5821b796&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-15&amp;pro=1</t>
+          <t>https://www.etsy.com/listing/1777988101/vintage-kite-cut-green-moss-agate?click_key=0bb68d76aaa58edb68731fefe1d4ec08b2cbc59a%3A1777988101&amp;click_sum=be92dd33&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-15&amp;pro=1&amp;sts=1</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>(10,533)</t>
+          <t>(9,342)</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/22438258/r/il/0a835f/6403075806/il_340x270.6403075806_lxr8.jpg</t>
+          <t>https://i.etsystatic.com/14110719/c/1388/1103/35/124/il/ab380f/3712342121/il_340x270.3712342121_fl43.jpg</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Oval-Cut Solitaire Ring – 14K Gold Bezel Set Ring with Split Shank Design – Elegant Engagement or Promise Ring</t>
+          <t>Nature Inspired Bee,Fox and Dinosaur Claws Engagement Ring w/ Oval Cut Montana Sapphire,Teal Sapphire engagement Ring,Unique Engagement Ring</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>421.64</t>
+          <t>3,600.00</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/4304003605/oval-cut-solitaire-ring-14k-gold-bezel?click_key=9da4f0c1b62d42a11247dbebb2f65541edeb18c5%3A4304003605&amp;click_sum=de3ecbc1&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765482-1-16&amp;pro=1&amp;frs=1</t>
+          <t>https://www.etsy.com/listing/4307727574/nature-inspired-beefox-and-dinosaur?click_key=07094de73745d9b87a7ff54272b9287b1eb77acd%3A4307727574&amp;click_sum=562446c8&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-16</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>(18)</t>
+          <t>(81)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/45784057/r/il/28e5cf/6854902636/il_340x270.6854902636_lcpc.jpg</t>
+          <t>https://i.etsystatic.com/22798206/r/il/ebf158/6921723911/il_340x270.6921723911_38pk.jpg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CH In Box 925 Silver Cross Pendant necklace adjustable chain gothic style Y2K rosary Jewelry Birthday Gift 60CM</t>
+          <t>In Box CH Silver Punk cross bracelet gothic style Jewelry cross rosary letter chain Birthday Gift</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>27.79</t>
+          <t>32.98</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1893318079/ch-in-box-925-silver-cross-pendant?click_key=958e1e4e131307b4e6252f48570b21c9ca03318e%3A1893318079&amp;click_sum=0ccfc689&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-37&amp;pro=1&amp;sts=1&amp;content_source=958e1e4e131307b4e6252f48570b21c9ca03318e%253A1893318079</t>
+          <t>https://www.etsy.com/listing/4299184491/in-box-ch-silver-punk-cross-bracelet?click_key=ecb3f040d9cf2b8aa628f71b8fa5586238edcffa%3A4299184491&amp;click_sum=20c2ff45&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-37&amp;pro=1&amp;content_source=ecb3f040d9cf2b8aa628f71b8fa5586238edcffa%253A4299184491</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>(445)</t>
+          <t>(6)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/56470180/r/il/e6329d/6790363477/il_340x270.6790363477_7xsi.jpg</t>
+          <t>https://i.etsystatic.com/58053909/r/il/7833b0/6830614112/il_340x270.6830614112_909z.jpg</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Personalized Necklace - Engraved Necklace - Custom Engraving Necklace - Family Necklace - Stainless Steel Necklace - Name Necklace - K530</t>
+          <t>CH In Box 925 Silver Cemetery zircon Cross silver rings Dagger ring man woman neutral couple Ring punk y2k opium Gothic designer jewelry</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>31.65</t>
+          <t>31.56</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1223037163/personalized-necklace-engraved-necklace?click_key=05764bef270adec613c9dfa970006abcb7b2c8e5%3A1223037163&amp;click_sum=7c055954&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-38&amp;etp=1&amp;sts=1&amp;content_source=05764bef270adec613c9dfa970006abcb7b2c8e5%253A1223037163</t>
+          <t>https://www.etsy.com/listing/4304973761/ch-in-box-925-silver-cemetery-zircon?click_key=e1f6bf0c011cf74f2b625c315adcc8d94ae51ee1%3A4304973761&amp;click_sum=61a1f4cb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-38&amp;pro=1&amp;frs=1&amp;content_source=e1f6bf0c011cf74f2b625c315adcc8d94ae51ee1%253A4304973761</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>(23,866)</t>
+          <t>(1)</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/8683017/r/il/45f145/3887802219/il_340x270.3887802219_j4va.jpg</t>
+          <t>https://i.etsystatic.com/53924353/r/il/ac36c6/6859717574/il_340x270.6859717574_gto1.jpg</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>925 Silver or 14K Gold Dainty name necklace with desired name made of real 925 Silver or 14K Gold Gift for Mom Mother's Day gift</t>
+          <t>Crystal Sun and Moon Earrings, Dangle Earrings, Wire Wrap Crystal Earrings</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>27.00</t>
+          <t>15.78</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1029635549/925-silver-or-14k-gold-dainty-name?click_key=0161a9f3ec8743850717ea3314adc07dc0d819b9%3A1029635549&amp;click_sum=682825e9&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-39&amp;pro=1&amp;sts=1&amp;content_source=0161a9f3ec8743850717ea3314adc07dc0d819b9%253A1029635549</t>
+          <t>https://www.etsy.com/listing/1295706184/crystal-sun-and-moon-earrings-dangle?click_key=67706e6917ce1bd62369d6c567fef4927822077c%3A1295706184&amp;click_sum=3f0cb329&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-39&amp;pro=1&amp;sts=1&amp;content_source=67706e6917ce1bd62369d6c567fef4927822077c%253A1295706184</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>(9,831)</t>
+          <t>(1,177)</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/21178078/c/1785/1419/557/1045/il/1b994d/3719278916/il_340x270.3719278916_duf2.jpg</t>
+          <t>https://i.etsystatic.com/27245498/r/il/5f4a6f/4237309847/il_340x270.4237309847_jnm5.jpg</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Trinket Dish, Watercolor Flower Ring Dish, Birthday Jewelry Dish Gift for Friend, Wedding Bridesmaid Gift</t>
+          <t>Mystery Jewelry Jars, Vintage Style Mystery Jewelry Jar, Mystery Jewelry Lot of Necklaces Pendants Bracelets Rings Earrings, Gift for Her</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8.79</t>
+          <t>14.57</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1773953582/personalised-birth-flower-trinket-dish?click_key=b44f040e582dddf5aa1248b2ea59a16e19ea8d7e%3A1773953582&amp;click_sum=889ab31f&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-40&amp;pro=1&amp;sts=1&amp;content_source=b44f040e582dddf5aa1248b2ea59a16e19ea8d7e%253A1773953582</t>
+          <t>https://www.etsy.com/listing/1882002443/mystery-jewelry-jars-vintage-style?click_key=336bea60fe608e31b326b31ff39be42d4ff05b3f%3A1882002443&amp;click_sum=a602eeec&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-40&amp;pro=1&amp;content_source=336bea60fe608e31b326b31ff39be42d4ff05b3f%253A1882002443</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>(884)</t>
+          <t>(165)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/53792712/c/1398/1398/351/351/il/2d7d24/6299541960/il_340x270.6299541960_20sf.jpg</t>
+          <t>https://i.etsystatic.com/55418552/r/il/101a03/6851948095/il_340x270.6851948095_ha47.jpg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>necklace trendy marine mesh sautoir necklace in adjustable gold stainless steel</t>
+          <t>Gold Earrings, Gold Disc Earrings, Silver Earrings, Circle Earrings, Handmade Jewelry, Gold Jewelry Gift, Round Earrings, Gold Stud Earrings</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>34.11</t>
+          <t>37.29</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1862377677/necklace-trendy-marine-mesh-sautoir?click_key=5136e8f45bfcbcb3238aa7f7cc169406ae02d115%3A1862377677&amp;click_sum=746686f4&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-41&amp;frs=1&amp;bes=1&amp;sts=1&amp;content_source=5136e8f45bfcbcb3238aa7f7cc169406ae02d115%253A1862377677</t>
+          <t>https://www.etsy.com/listing/1128664829/gold-earrings-gold-disc-earrings-silver?click_key=3d39b0ec2628066f0b852035d08b2468553050a0%3A1128664829&amp;click_sum=e338fe92&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-41&amp;etp=1&amp;sts=1&amp;content_source=3d39b0ec2628066f0b852035d08b2468553050a0%253A1128664829</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>(313)</t>
+          <t>(3,514)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/41158284/r/il/93ea02/6759154320/il_340x270.6759154320_jp2l.jpg</t>
+          <t>https://i.etsystatic.com/17763464/c/1626/1292/55/291/il/860a78/3543836963/il_340x270.3543836963_ebw0.jpg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Gold Enamel Mini Cross Necklace, Tiny Cross Necklace, Religious Necklace, Enamel Necklace, Christian Gift for her, Christmas Gift</t>
+          <t>Leather travel jewelry case,Leather jewelry storage,Personalized jewelry organizer,Leather jewelry roll,Personalized jewelry roll</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>15.47</t>
+          <t>48.60</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1811620349/gold-enamel-mini-cross-necklace-tiny?click_key=86c56fa0b023dff1df2c4f078687c6700ede11e0%3A1811620349&amp;click_sum=94ce5aae&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-42&amp;pro=1&amp;sts=1&amp;content_source=86c56fa0b023dff1df2c4f078687c6700ede11e0%253A1811620349</t>
+          <t>https://www.etsy.com/listing/1376195359/leather-travel-jewelry-caseleather?click_key=90f51fc190850b61be0b632faed0a4b2473c8da1%3A1376195359&amp;click_sum=97c6e4e5&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-42&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=90f51fc190850b61be0b632faed0a4b2473c8da1%253A1376195359</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>(3,055)</t>
+          <t>(1,890)</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/55368172/r/il/a3c6a8/6358770680/il_340x270.6358770680_cisx.jpg</t>
+          <t>https://i.etsystatic.com/19642071/r/il/cd4ad6/4451985490/il_340x270.4451985490_blz6.jpg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Photo Projection Necklace, Gift for Her, Birthstone Necklace, Personalized Photo Necklace, Memorial Gift, Valentine Day Gift, Mom Necklace</t>
+          <t>Against the Current Sterling Silver Ring | Adjustable Blue Fish Ring for Men &amp; Women | Unique Swimming Fish Design | Symbolic Jewelry Gift</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>23.60</t>
+          <t>33.72</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1496953538/photo-projection-necklace-gift-for-her?click_key=42400a074f4e027fafb7988bf324c0cada5de70d%3A1496953538&amp;click_sum=d319d264&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-43&amp;pro=1&amp;frs=1&amp;content_source=42400a074f4e027fafb7988bf324c0cada5de70d%253A1496953538</t>
+          <t>https://www.etsy.com/listing/1854693866/against-the-current-sterling-silver-ring?click_key=c001347597cbc3d7c78d37640dd273902b4ff8fa%3A1854693866&amp;click_sum=afab10c7&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-43&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=c001347597cbc3d7c78d37640dd273902b4ff8fa%253A1854693866</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>(8,781)</t>
+          <t>(31)</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/27946180/c/2666/2110/0/397/il/262003/5034148022/il_340x270.5034148022_cjjb.jpg</t>
+          <t>https://i.etsystatic.com/56974458/r/il/63d1fd/6617860330/il_340x270.6617860330_kz7v.jpg</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CH In Box 925 Silver Vintage Double Cross Pedant necklace chrome choke chain gothic style Y2K Jewelry Birthday Gift</t>
+          <t>Forget-Me-Not Necklace, Necklace for Women, Real Pressed Flower Jewerly, Forgetmenot, Flower Resin Jewelry, Bridesmaid Gifts, Gift for Her</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>27.79</t>
+          <t>18.69</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1879207338/ch-in-box-925-silver-vintage-double?click_key=fbc826d3752fa17d7abe80a39111142eba9ca054%3A1879207338&amp;click_sum=ca4ae2a3&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-44&amp;pro=1&amp;sts=1&amp;content_source=fbc826d3752fa17d7abe80a39111142eba9ca054%253A1879207338</t>
+          <t>https://www.etsy.com/listing/1774008366/forget-me-not-necklace-necklace-for?click_key=7abf4adb1f4ec8f9b2c6b3c48e7f16cd0944ec5f%3A1774008366&amp;click_sum=61eafc36&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-44&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=7abf4adb1f4ec8f9b2c6b3c48e7f16cd0944ec5f%253A1774008366</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>(445)</t>
+          <t>(1,928)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/56470180/r/il/1fed11/6790834913/il_340x270.6790834913_pplk.jpg</t>
+          <t>https://i.etsystatic.com/50890964/r/il/b7f1ae/6244433320/il_340x270.6244433320_4cf4.jpg</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>14K Gold Heart Locket Necklace,Heart Locket Necklace with Photo,Gold Vintage Heart Locket Necklace,Locket that Opens,Gift for MOM</t>
+          <t>Billie Eilish Blohsh Inspired Pendant Stainless Steel And Alloy Necklace</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>18.26</t>
+          <t>15.30</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1712871891/14k-gold-heart-locket-necklaceheart?click_key=8fcd49e225866be111314c26a01b604629645a8b%3A1712871891&amp;click_sum=05efd097&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-45&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=8fcd49e225866be111314c26a01b604629645a8b%253A1712871891</t>
+          <t>https://www.etsy.com/listing/1898349213/billie-eilish-blohsh-inspired-pendant?click_key=348ebec74056be580e56b2df724559907c14bfd3%3A1898349213&amp;click_sum=0e6ef5cb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-45&amp;pro=1&amp;content_source=348ebec74056be580e56b2df724559907c14bfd3%253A1898349213</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>(978)</t>
+          <t>(26)</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/49164871/c/1333/1058/416/575/il/dc6881/5924693700/il_340x270.5924693700_3ihj.jpg</t>
+          <t>https://i.etsystatic.com/50765934/r/il/daedea/6791549852/il_340x270.6791549852_mggb.jpg</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>18K Gold Filled Bracelets,Paperclip Chain,Herringbone Chain,Rope,Snake Chain Bracelet,Everyday Bracelet,Dainty Bracelet,Minimalist Bracelet</t>
+          <t>Italian Bracelet,Custom silver Italy Charms,Personalized Italian Bracelet,Vintage Jewelry Gifts for Her,Birthday gift,Christmas gift</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>15.99</t>
+          <t>20.35</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1811798767/18k-gold-filled-braceletspaperclip?click_key=989beb698a2c2db332935429ce644800b21b72a7%3A1811798767&amp;click_sum=0b236be5&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-46&amp;pro=1&amp;sts=1&amp;content_source=989beb698a2c2db332935429ce644800b21b72a7%253A1811798767</t>
+          <t>https://www.etsy.com/listing/1863639536/italian-braceletcustom-silver-italy?click_key=6b62e87dd9c51189ff12f1bd812a1b52cabc826e%3A1863639536&amp;click_sum=0424af10&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-46&amp;pro=1&amp;sts=1&amp;content_source=6b62e87dd9c51189ff12f1bd812a1b52cabc826e%253A1863639536</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>(2,828)</t>
+          <t>(51)</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/51464338/r/il/6ca537/6407812703/il_340x270.6407812703_7pp9.jpg</t>
+          <t>https://i.etsystatic.com/35651222/r/il/24c105/6710768929/il_340x270.6710768929_jvfd.jpg</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>925 Sterling Silver Ring for Men, Women / Hammered or Smooth / Custom Engraving / Mens Sterling Silver Ring / Silver Band / 5mm</t>
+          <t>Pandora Beaded Bracelet, European Charm Bracelets, S925 sterling silver heart clasp snake chain bracelet, Birthday gift for girlfriend</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>19.14</t>
+          <t>28.99</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1471336398/925-sterling-silver-ring-for-men-women?click_key=e4b6cf7f4acd5d6f1835a24f3a94f3f191dec9d7%3A1471336398&amp;click_sum=2c5b4d50&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-47&amp;pro=1&amp;content_source=e4b6cf7f4acd5d6f1835a24f3a94f3f191dec9d7%253A1471336398</t>
+          <t>https://www.etsy.com/listing/1879251072/pandora-beaded-bracelet-european-charm?click_key=07fbbf24ff8a8f4a33f30183487af5dcb259a6e8%3A1879251072&amp;click_sum=eec55a06&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-47&amp;pro=1&amp;content_source=07fbbf24ff8a8f4a33f30183487af5dcb259a6e8%253A1879251072</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>(2,424)</t>
+          <t>(62)</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/35258625/c/1500/1192/294/506/il/4508b0/4929948562/il_340x270.4929948562_8ugj.jpg</t>
+          <t>https://i.etsystatic.com/51978889/r/il/d9d88f/6742749410/il_340x270.6742749410_6gt5.jpg</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Single Real Pearl Necklace, Freshwater Pearl Pendent Necklace, Bridal Jewelry, Wedding Necklace, Christmas Necklace, Bridesmaid Gift for Her</t>
+          <t>If Friends were Flowers I'd Pick You Ring Dish,Personalized Birth Flower Jewelry Dish,Floral Trinket Dish for Friend,Birthday Gift for BFF</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>18.90</t>
+          <t>8.95</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1734924289/single-real-pearl-necklace-freshwater?click_key=a459d87f71dadc59946c34826e35e53d881a210b%3A1734924289&amp;click_sum=cce3603d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-765483-1-48&amp;pro=1&amp;sts=1&amp;content_source=a459d87f71dadc59946c34826e35e53d881a210b%253A1734924289</t>
+          <t>https://www.etsy.com/listing/1813761409/if-friends-were-flowers-id-pick-you-ring?click_key=a37ca940f7d23bd5ebd174bc7bdc440bfadf7c2b%3A1813761409&amp;click_sum=01da85b6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-48&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=a37ca940f7d23bd5ebd174bc7bdc440bfadf7c2b%253A1813761409</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>(13,931)</t>
+          <t>(2,634)</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://i.etsystatic.com/35046319/c/1680/1680/125/44/il/0f6c86/6636376306/il_340x270.6636376306_rp9h.jpg</t>
+          <t>https://i.etsystatic.com/48621519/c/1785/1785/107/81/il/a655af/6417461479/il_340x270.6417461479_pi4e.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Riverbed Wave Ring. 18K Gold Vermeil over Sterling Silver &amp; Green Enamel. Adjustable.</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>58.33</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1890762377/riverbed-wave-ring-18k-gold-vermeil-over?click_key=f21a040358e9c515e80c29a441fb47e7e88ec238%3A1890762377&amp;click_sum=735f36a1&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-1&amp;sca=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>(42,538)</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/6401969/r/il/bae740/6765875526/il_340x270.6765875526_60db.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Peridot earrings green earrings August birthstone jewelry Personalized Dangle Earrings Custom Birthstone Earrings birthday gift for her</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>29.32</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/90776791/peridot-earrings-green-earrings-august?click_key=30580b4770baca07e477a8f8be3936acaa9cc1f4%3A90776791&amp;click_sum=d032d245&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-2&amp;pro=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>(16,278)</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/6666729/c/782/621/0/287/il/46a4bc/6061329099/il_340x270.6061329099_an55.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>14K Yellow Gold Floral Ring with Mother of Pearl &amp; 0.96 Ct Green Peridot Gemstone CGL Certified Elegant Jewelry adjustable Made To Order</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>531.00</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4303764453/14k-yellow-gold-floral-ring-with-mother?click_key=f9a170e81004032c8c27fe38afade16b6c6be726%3A4303764453&amp;click_sum=f2aebccf&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-3&amp;pro=1&amp;frs=1</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/57683402/r/il/79b808/6895208857/il_340x270.6895208857_jzm4.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Emerald Ring, Handmade Women's Ring, Turkish Handmade Ring, Authentic Ring, Ottoman Ring, Ladies Ring, 925k Sterling Silver, Cubic Zircon</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>42.00</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/977242742/emerald-ring-handmade-womens-ring?click_key=e260881bac8e01ab8d42d615d442bc6a4fe3ad4b%3A977242742&amp;click_sum=8cd08bc3&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-4&amp;pro=1</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>(10,361)</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/22806411/c/1342/1067/218/189/il/65d520/3106195309/il_340x270.3106195309_d8y8.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Coquette Fairycore Themed Mystery Jewelry Jar, Curated Jewelry Jars of Necklaces, Bracelets, Rings &amp; Earrings, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>14.57</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4303224938/coquette-fairycore-themed-mystery?click_key=c596ff9e5dfe6fb3914fb4b93d905c99fdc44c99%3A4303224938&amp;click_sum=dcd16ab9&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-1&amp;pro=1&amp;content_source=c596ff9e5dfe6fb3914fb4b93d905c99fdc44c99%253A4303224938</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>(165)</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/55418552/r/il/7e93ad/6871013788/il_340x270.6871013788_s8eq.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Mystery Jewelry Jar - Modern Minimalist Theme, Curated Jewelry Jars of Necklaces, Bracelets, Rings &amp; Earrings, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>14.57</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1814825794/mystery-jewelry-jar-modern-minimalist?click_key=d0f9de7ba80eb8de3283154678368daa84bf983b%3A1814825794&amp;click_sum=225a3b4b&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-2&amp;pro=1&amp;content_source=d0f9de7ba80eb8de3283154678368daa84bf983b%253A1814825794</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>(165)</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/55418552/r/il/64296c/6919382099/il_340x270.6919382099_olei.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Mystery Jewelry Jars, Witchy Whimsical Gothic Jewelry Jar, Mystery Jewelry Lot of Necklaces Pendants Bracelets Rings Earrings, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14.57</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4302282840/mystery-jewelry-jars-witchy-whimsical?click_key=7ac3e28109134db857f6fb68eaf4301f0564f7d8%3A4302282840&amp;click_sum=4311c83a&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-3&amp;pro=1&amp;content_source=7ac3e28109134db857f6fb68eaf4301f0564f7d8%253A4302282840</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>(165)</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/55418552/r/il/94ad99/6893941603/il_340x270.6893941603_4oaj.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Mystery Jewellery Jars</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>33.34</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4304484065/mystery-jewellery-jars?click_key=ec4005a2a8e55fa78cb1a8b7adb57e85aadda601%3A4304484065&amp;click_sum=35278339&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-4&amp;cns=1&amp;content_source=ec4005a2a8e55fa78cb1a8b7adb57e85aadda601%253A4304484065</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>(41)</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/56707580/r/il/f1a992/6857333856/il_340x270.6857333856_rwfo.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Vintage Gold Watch Bracelet,Retro Timepiece Jewelry,Elegant Tiger Eye Clock Bracelet,Unique Handmade Fashion Accessory,Luxury Jewelry Gift</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>26.30</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4297824541/vintage-gold-watch-braceletretro?click_key=21bc9e0b51b1208748c851a9222ed917b6f9f75f%3A4297824541&amp;click_sum=50aaf822&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-5&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=21bc9e0b51b1208748c851a9222ed917b6f9f75f%253A4297824541</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>(85)</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/53454032/r/il/ec1c39/6824047770/il_340x270.6824047770_fjpd.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Custom Name Necklace, 18K Gold Plated Name Necklace, Personalized Name Necklace, Birthday Gift for Her, Mother's Day Gift, Gift for Mom</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>15.27</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1413455244/custom-name-necklace-18k-gold-plated?click_key=ab3a07bdc289f3abf4462cdddca5884bab39cf94%3A1413455244&amp;click_sum=ac666f10&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-6&amp;pro=1&amp;sts=1&amp;content_source=ab3a07bdc289f3abf4462cdddca5884bab39cf94%253A1413455244</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>(41,773)</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/34379934/c/2000/1589/0/264/il/628644/4796937795/il_340x270.4796937795_qnr6.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Custom Italian Charm Bracelet, Gold Italy Charms Bracelet, Vintage Best Friend Bracelet, Handmade Italian Watch Bracelets for Women Gifts</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>16.89</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1873039828/custom-italian-charm-bracelet-gold-italy?click_key=ee4b62be2ea4d8bb174a4fcfdf2b2daf0c8b8986%3A1873039828&amp;click_sum=f4c1a16d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-7&amp;pro=1&amp;sts=1&amp;content_source=ee4b62be2ea4d8bb174a4fcfdf2b2daf0c8b8986%253A1873039828</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>(125)</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/11609255/c/1724/1724/108/115/il/536f9e/6710479364/il_340x270.6710479364_lwo1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>VVS1 Tennis Bracelet, 2-4MM Moissanite &amp; 925 Sterling Silver, Sparkling Moissanite, Passes Diamond Tester</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>67.45</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1853948798/vvs1-tennis-bracelet-2-4mm-moissanite?click_key=e847394a3bd9a76ceb57e5e55e1684a449e02e12%3A1853948798&amp;click_sum=bc4672b3&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-8&amp;pro=1&amp;frs=1&amp;content_source=e847394a3bd9a76ceb57e5e55e1684a449e02e12%253A1853948798</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>(29)</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/56024009/r/il/8e110b/6741930986/il_340x270.6741930986_kerr.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Natural Rainbow Moonstone 925 Sterling Silver Oval Shape Adjustable Bracelet, Gemstone Jewelry, Tennis Bracelet, Gift For Her, Gift For Love</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14.15</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1310205516/natural-rainbow-moonstone-925-sterling?click_key=c1618432a06024897693ec3927371e18694090b4%3A1310205516&amp;click_sum=681aa697&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-9&amp;pro=1&amp;content_source=c1618432a06024897693ec3927371e18694090b4%253A1310205516</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>(8,748)</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/37557222/r/il/fa25a9/4247357962/il_340x270.4247357962_kv3m.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Personalized Italian Bracelet, Custom Gold Italy Charms, Gold Italian Bracelet, Italy Charms, Gold Italian Charm Bracelet, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>24.42</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1798191819/personalized-italian-bracelet-custom?click_key=47fe96df04b7e560b8de063c005766be59e9b54b%3A1798191819&amp;click_sum=1d34d9bf&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-10&amp;pro=1&amp;sts=1&amp;content_source=47fe96df04b7e560b8de063c005766be59e9b54b%253A1798191819</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>(829)</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/53495552/r/il/59bdad/6338540867/il_340x270.6338540867_htw1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Silver Italian Bracelets, 18 Links Italian Bracelets, Vintage Italian Bracelets, Personalized Italian Bracelets</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>15.60</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1848633141/silver-italian-bracelets-18-links?click_key=2cb6a7e919f0ce6bb5f9f296b0cb86654ce6db39%3A1848633141&amp;click_sum=bc2121cf&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-11&amp;pro=1&amp;content_source=2cb6a7e919f0ce6bb5f9f296b0cb86654ce6db39%253A1848633141</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>(344)</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/53633588/r/il/07335b/6523810440/il_340x270.6523810440_t87i.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Blohsh Symbol Dog Tag Necklace｜High Quality Stainless Steel Polished｜Waterproof and Rustproof Design｜Men's and Women's Fashion Accessories</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>10.23</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4298141396/blohsh-symbol-dog-tag-necklacehigh?click_key=2423b555f1811f7dc0d1b776549648d81bf98319%3A4298141396&amp;click_sum=06721012&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-12&amp;pro=1&amp;content_source=2423b555f1811f7dc0d1b776549648d81bf98319%253A4298141396</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/59133224/r/il/c3b910/6825611024/il_340x270.6825611024_brfx.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Adorable Kids Birthstone Necklace Personalized Birthday Gift for Little Girls Dainty Birthday Gift Gemstone Charm Necklace for Child</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>43.00</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1515508065/adorable-kids-birthstone-necklace?click_key=07a5fd7460664c55b63acadfde4a2d370071d37e%3A1515508065&amp;click_sum=3150b01d&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-5&amp;bes=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>(21,234)</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/10230423/r/il/9249dd/5408070742/il_340x270.5408070742_oebv.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>0.30 Ct Diamond Stud Earring Round Diamond Solitaire Earrings 14k Yellow Gold 14K White Gold 14K Rose gold</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>29.98</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/551905860/030-ct-diamond-stud-earring-round?click_key=fd710bbb9d2ecc3904a174d82e56b9a97ca1dc61%3A551905860&amp;click_sum=31b74b9e&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-6&amp;bes=1</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>(2,381)</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/15822554/c/1829/1453/176/246/il/bcee16/1413433427/il_340x270.1413433427_pqgk.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Travel &amp; Storage Watch Roll For 4 Watches With Stand Function - Watch Box For Storage - Epsom Leather - Men's Gift - Color: BLACK</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>474.28</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1060896422/travel-storage-watch-roll-for-4-watches?click_key=1884d1a8a3f3a2ad13f63ddb39566efdc0cccc34%3A1060896422&amp;click_sum=c1fdb05a&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-7&amp;frs=1</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>(247)</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/13579477/r/il/2a77b5/3291321912/il_340x270.3291321912_bsbr.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Vintage Lab Created Emerald 10K Rose Gold Engagement Ring Art Deco Nature Inspired Leaf Wedding Ring Gift For Women Promise Moissanite Ring</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>116.20</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1621460129/vintage-lab-created-emerald-10k-rose?click_key=1667f73d87c720518f8aa2c949a2ed2cf57af834%3A1621460129&amp;click_sum=7a94d986&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-8&amp;pro=1&amp;frs=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>(348)</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/43099566/r/il/97dc80/5547706040/il_340x270.5547706040_jcsq.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Pink Peach Blossom Open Ring,Ring for women,Fashion jewelry,Gift for her Rose Gold Plating</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>20.52</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1805128091/pink-peach-blossom-open-ringring-for?click_key=ef0ae277d55930f83823a04fad48d28e5819cf00%3A1805128091&amp;click_sum=088b30cb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-13&amp;pro=1&amp;frs=1&amp;content_source=ef0ae277d55930f83823a04fad48d28e5819cf00%253A1805128091</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>(296)</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/52310599/r/il/9001c9/6325150620/il_340x270.6325150620_hxsn.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Custom Birthflower Necklace with Birthstone, Family Birth Flower Necklacce, Birth Month Necklace, Bridesmaids Gift for Her, Mothers Day Gift</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>13.88</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1706218238/custom-birthflower-necklace-with?click_key=9f9b17059aab6d4f61e202a05d9ea6592b74f0f2%3A1706218238&amp;click_sum=a349f296&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-14&amp;pro=1&amp;sts=1&amp;content_source=9f9b17059aab6d4f61e202a05d9ea6592b74f0f2%253A1706218238</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>(1,595)</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/51686135/c/1123/892/476/758/il/b391c7/6018489414/il_340x270.6018489414_5ijh.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Pressed Flower Jewelry Set – Real Pansy Pendant and Earrings – Botanical Glass Jewelry – Nature Gift for Her – Violet Flower Jewelry</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>57.00</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4300565424/pressed-flower-jewelry-set-real-pansy?click_key=a7791f6c56c92c5567ed8b157e416b8d4af8d33c%3A4300565424&amp;click_sum=513905fe&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-15&amp;pro=1&amp;content_source=a7791f6c56c92c5567ed8b157e416b8d4af8d33c%253A4300565424</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>(716)</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/19164025/r/il/fd87ee/6842562520/il_340x270.6842562520_3nw2.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>14G Dagger Industrial Barbell/Retro textured Industrial Jewelry/Industrial Piercing/Scaffold Jewelry/Industrial Earring/Staight Barbell/Gift</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>10.49</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4304168382/14g-dagger-industrial-barbellretro?click_key=8e00cf02dba45f43d08a71a76a03a478a97b64b1%3A4304168382&amp;click_sum=0d214499&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-16&amp;pro=1&amp;sts=1&amp;content_source=8e00cf02dba45f43d08a71a76a03a478a97b64b1%253A4304168382</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>(88,399)</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/21623448/c/1834/1834/82/82/il/d05fed/6855794862/il_340x270.6855794862_9mtp.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>18K Gold Filled Bracelets,Paperclip Chain,Herringbone Chain,Rope,Snake Chain Bracelet,Everyday Bracelet,Dainty Bracelet,Minimalist Bracelet</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>15.99</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1811798767/18k-gold-filled-braceletspaperclip?click_key=0119f2eaa69e8da6892f4511adb0a4d51d4ed88a%3A1811798767&amp;click_sum=e9932098&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-17&amp;pro=1&amp;sts=1&amp;content_source=0119f2eaa69e8da6892f4511adb0a4d51d4ed88a%253A1811798767</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>(2,914)</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/51464338/r/il/6ca537/6407812703/il_340x270.6407812703_7pp9.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Heart and Sword Couple Necklace Set - 2pcs Silver Plated Necklaces - Matching His and Hers Jewelry</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>19.45</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1836962223/heart-and-sword-couple-necklace-set-2pcs?click_key=d876ba2fb695127ccbdb4bb27889130a9babcf2c%3A1836962223&amp;click_sum=2af1b699&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-18&amp;pro=1&amp;content_source=d876ba2fb695127ccbdb4bb27889130a9babcf2c%253A1836962223</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>(117)</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/49738791/r/il/9622fe/6528189735/il_340x270.6528189735_ak2j.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Green Copper Turquoise Bangle, 925 Silver Bangle, Handmade Bangle, Women Bangle, Adjustable Bangle, Everyday Bangle, Silver Bracelet Jewelry</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>18.01</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1365985292/green-copper-turquoise-bangle-925-silver?click_key=9df7e5605dc2d371ae376ac2d67e05ef50d2b689%3A1365985292&amp;click_sum=8e472563&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-19&amp;pro=1&amp;content_source=9df7e5605dc2d371ae376ac2d67e05ef50d2b689%253A1365985292</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>(8,748)</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/37557222/r/il/d8a2eb/4463869778/il_340x270.4463869778_2sv9.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2 Names Necklace with Heart, Personalized Couple Names Necklace, Name Necklace Gift for Mom, Two Name Necklace, Gift for Wife, Mom of Two</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>20.08</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1777488475/2-names-necklace-with-heart-personalized?click_key=64820679e7a5f2bfc925e9ac9e68bd5f7c8af710%3A1777488475&amp;click_sum=ca38b20d&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-20&amp;pro=1&amp;frs=1&amp;content_source=64820679e7a5f2bfc925e9ac9e68bd5f7c8af710%253A1777488475</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>(770)</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/53277887/c/2000/2000/0/0/il/37b131/6514071229/il_340x270.6514071229_7dpi.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Italian Bracelet,Custom silver Italy Charms,Personalized Italian Bracelet,Evil Eye Charms,Jewelry Gifts for Her,Birthday gift,Christmas gift</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>21.09</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1787047600/italian-braceletcustom-silver-italy?click_key=96fd252e30f5f0098e867d913491535bbbb66ecf%3A1787047600&amp;click_sum=a0f7cc24&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-21&amp;pro=1&amp;sts=1&amp;content_source=96fd252e30f5f0098e867d913491535bbbb66ecf%253A1787047600</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>(777)</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/52861665/r/il/63a3fd/6353940707/il_340x270.6353940707_eqs7.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Iced Out Personalized Big Name Pendant with 12mm Cuban Link Chain,Custom Name Necklace,Custom Chain,Hiphop Jewelry,Custom Birthday Gifts</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>27.60</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1683162610/iced-out-personalized-big-name-pendant?click_key=84df93e7f3b3d723ad2ecd87891c045302cb529f%3A1683162610&amp;click_sum=ba913d06&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-22&amp;pro=1&amp;sts=1&amp;content_source=84df93e7f3b3d723ad2ecd87891c045302cb529f%253A1683162610</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>(2,420)</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/25298655/c/2992/2376/0/76/il/85a58a/5901019163/il_340x270.5901019163_3cuh.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>18K Gold Filled Chain Necklace,Curb,Figaro,Rope,Paperclip Chain,Herringbone Chain,twist Chain,Gift For Her,Gift for him, Mother’s Day Gifts</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>22.09</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1624025579/18k-gold-filled-chain?click_key=0a6b0599c20b3a92ce1e7e5fd0cacb12e3619110%3A1624025579&amp;click_sum=25a30898&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-23&amp;pro=1&amp;frs=1&amp;content_source=0a6b0599c20b3a92ce1e7e5fd0cacb12e3619110%253A1624025579</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>(3,268)</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/37567900/r/il/901062/5557563622/il_340x270.5557563622_4gjd.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Cloisonne Bracelets, Vintage Green/Red/Purple/Blue/Pink/Yellow Enamel Flowers Bracelets, Anniversary Gift, Birthday Gift, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>12.68</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1883423978/cloisonne-bracelets-vintage?click_key=4f48fb370df219942befb090140203572dea029c%3A1883423978&amp;click_sum=9cd4394c&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-24&amp;pro=1&amp;frs=1&amp;content_source=4f48fb370df219942befb090140203572dea029c%253A1883423978</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>(6)</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/54138066/r/il/ddef71/6812004839/il_340x270.6812004839_mxzm.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Mens Bracelet with Stainless Steel Rings • Adjustable Bracelet Men • Waterproof Bracelet Women • Mens Jewelry • Gift For Him</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>16.35</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1704505485/mens-bracelet-with-stainless-steel-rings?click_key=2e102bc59b01445f4168bb8c51e573978cf12f5e%3A1704505485&amp;click_sum=284fa48f&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-9&amp;etp=1</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>(32,683)</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/13238741/c/2419/1923/268/454/il/67d10e/5877699290/il_340x270.5877699290_kibf.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>14K Gold Diamond Cross Necklace for Women | Minimalist Diamond Cross Pendant | 14K Gold Jewelry | Perfect Graduation Gift</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>184.00</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1806364223/14k-gold-diamond-cross-necklace-for?click_key=4ecf77b61a7bea8b444e77506a6d63c5f49f06e7%3A1806364223&amp;click_sum=bb19e7fe&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-10&amp;pro=1&amp;frs=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>(19)</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/54432389/c/1388/1388/400/620/il/a9c600/6331474802/il_340x270.6331474802_om5t.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Carnelian Necklace, Gold Carnelian Pendant, Personalized Necklace Gift, Witchy Jewelry, Best Friend Gift, Unique Gift for Her</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>54.24</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4307066524/carnelian-necklace-gold-carnelian?click_key=1fd4326796facd9376546de8d2e30e61f531dadf%3A4307066524&amp;click_sum=bae7dbe9&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-11</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>(4,458)</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/17842620/c/1301/1301/143/12/il/19c615/6870317496/il_340x270.6870317496_360x.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>14k Gold Dome Wedding Band / Yellow, Rose and White Gold Dome Ring / Matching Wedding Band for Women / Solid Gold Band Ring Sets</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>159.75</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1251774176/14k-gold-dome-wedding-band-yellow-rose?click_key=7e07434aef0d9dd9149e6818122dcdccac6e034f%3A1251774176&amp;click_sum=6bdee5c4&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-12&amp;pro=1&amp;frs=1</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>(2,152)</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/36471853/c/1804/1434/778/478/il/f3d666/4036768632/il_340x270.4036768632_67hz.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>18K Gold Filled Chain Necklace,Pearl Chain,Curb Chian,Box Chain,Paperclip Chain,Twist Chain,Dainty Chain,Gift for Her,Mothers Day Gifts</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>11.99</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1782276981/18k-gold-filled-chain-necklacepearl?click_key=7512c3a0ed8136f6a36032c9d8afe6a80d394561%3A1782276981&amp;click_sum=e86065e6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-25&amp;pro=1&amp;sts=1&amp;content_source=7512c3a0ed8136f6a36032c9d8afe6a80d394561%253A1782276981</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>(2,914)</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/51464338/r/il/ee68f9/6294619536/il_340x270.6294619536_69q2.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Labradorite Copper Pendant Copper Wire Wrapped Gemstone Pendant Handmade Copper Wire Jewelry Gift For Wife Labradorite Jewelry Wedding Gift</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>17.06</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1250123390/labradorite-copper-pendant-copper-wire?click_key=78da3d7a6fea1bcd9745c6a64cdb4c750aeaa464%3A1250123390&amp;click_sum=67f43c92&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-26&amp;pro=1&amp;frs=1&amp;content_source=78da3d7a6fea1bcd9745c6a64cdb4c750aeaa464%253A1250123390</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>(15,753)</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/10932069/r/il/f8d6d1/4042142991/il_340x270.4042142991_m6hb.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>18K Gold Chain Necklace/Cable Chain/Paperclip Chain/Twist Chain/Figaro/Curb Chain/Bead Chain/Blade Chain/Chain for kids/Mothers Day Gifts</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>11.87</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1802574426/18k-gold-chain-necklacecable?click_key=2b2c914da695b8a38776aaa664d23e33c8244e52%3A1802574426&amp;click_sum=d3a4ddd3&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-27&amp;pro=1&amp;frs=1&amp;content_source=2b2c914da695b8a38776aaa664d23e33c8244e52%253A1802574426</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>(62)</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/54758409/r/il/185c7e/6432383117/il_340x270.6432383117_icqr.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>925 Sterling Silver Rope Chain Necklace,Real Silver Chain,Silver Jewelry Chain Necklaces For Women And Mens ,Choker Chain, Chain for Pendant</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>22.22</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1740374254/925-sterling-silver-rope-chain?click_key=5339bb59ced00dcda2f37f5cc3c90d30e7449b71%3A1740374254&amp;click_sum=3f3ab6fb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-28&amp;pro=1&amp;frs=1&amp;content_source=5339bb59ced00dcda2f37f5cc3c90d30e7449b71%253A1740374254</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>(500)</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/52961888/r/il/04f3f3/6188504811/il_340x270.6188504811_56bw.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Upper arm cuff arm band spiral handmade made of brass, jewelry</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>18.30</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1696016225/upper-arm-cuff-arm-band-spiral-handmade?click_key=546f623ddfc4d0e1ff215cb1b0115ef18d3298f0%3A1696016225&amp;click_sum=c0213bf6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-29&amp;pro=1&amp;content_source=546f623ddfc4d0e1ff215cb1b0115ef18d3298f0%253A1696016225</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>(465)</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/39191393/r/il/218f84/5840542934/il_340x270.5840542934_1llm.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Arcane Pendant &amp; Keychain | Dual-Sided Blue Rose Design | VI, Jinx, Ekko Inspired | Perfect Gift for Fans, League of Legends Hextech cosplay</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>21.67</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4298325681/arcane-pendant-keychain-dual-sided-blue?click_key=6eb3f36d71f8f4073da7425bd4e52e79f97811f7%3A4298325681&amp;click_sum=4b217f4a&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-30&amp;pro=1&amp;frs=1&amp;content_source=6eb3f36d71f8f4073da7425bd4e52e79f97811f7%253A4298325681</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>(55)</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/56411742/r/il/269ede/6874531515/il_340x270.6874531515_pkws.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Ivan Cornejo, Ivan Cornejo Inspired, Ivan C Inspired Handmade Bracelets</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1861748200/ivan-cornejo-ivan-cornejo-inspired-ivan?click_key=24436b4f1e2add9f51988838159d9c75a3824667%3A1861748200&amp;click_sum=33fde49e&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-31&amp;content_source=24436b4f1e2add9f51988838159d9c75a3824667%253A1861748200</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>(964)</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/30749325/r/il/ed4ec4/6652934310/il_340x270.6652934310_c51g.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>14k Gold Emerald Heart Necklace, Minimalist Heart Shaped Emerald Love Pendant Necklace, Heart Cut Emerald Birthstone Jewelry, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1775155890/14k-gold-emerald-heart-necklace?click_key=8bfe5ee55c1b2883f76d7d1c9db139f3b416b9b7%3A1775155890&amp;click_sum=31d56f15&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-32&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=8bfe5ee55c1b2883f76d7d1c9db139f3b416b9b7%253A1775155890</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>(114)</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/51548529/c/1874/1874/495/562/il/dc2972/6249655746/il_340x270.6249655746_9fwx.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>handmade dew necklace "wave drops"</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>56.65</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1809936026/handmade-dew-necklace-wave-drops?click_key=25ffd30b6bc9abe2f01e1e5a28d9feef9ce80e09%3A1809936026&amp;click_sum=8938e008&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-33&amp;bes=1&amp;sts=1&amp;content_source=25ffd30b6bc9abe2f01e1e5a28d9feef9ce80e09%253A1809936026</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>(140)</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/55955607/r/il/adf9ee/6468934587/il_340x270.6468934587_tbuk.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>18K Gold Filled Chain Necklace, Curb ,Figaro, Dainty, Rope Chain, Valentines Day,Paperclip Chain,Snake Chain,Mothers Day Gift, Gift For Her</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>23.06</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1570883974/18k-gold-filled-chain-necklace-curb?click_key=dced132d0e7e18c824bc21f0bb282501ff2edfa6%3A1570883974&amp;click_sum=8f886f09&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-34&amp;pro=1&amp;frs=1&amp;content_source=dced132d0e7e18c824bc21f0bb282501ff2edfa6%253A1570883974</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>(948)</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/47300955/r/il/fe0595/5436560409/il_340x270.5436560409_kvws.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>8mm Adjustable Bangle Bracelet, Colorful Bangle Bracelet, Flower Pattern Enamel Bangle, Women's Bangle Bracelet, Floral Bangles</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>15.32</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1876267248/8mm-adjustable-bangle-bracelet-colorful?click_key=649f93ab479f677111d2b79a96d26d1aaab6bead%3A1876267248&amp;click_sum=4d9467de&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-35&amp;pro=1&amp;frs=1&amp;content_source=649f93ab479f677111d2b79a96d26d1aaab6bead%253A1876267248</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>(21)</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/57066309/r/il/c5e275/6818479806/il_340x270.6818479806_lq4l.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Handmade Birthstone Name Necklace, Personalized Name Necklace, Necklace with Birthstone, Christmas Gift for Her, Women Gift for Wedding</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>17.09</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1773370947/handmade-birthstone-name-necklace?click_key=1fc82e51759cd729859b13944268283526c45c7f%3A1773370947&amp;click_sum=62cbb530&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-36&amp;pro=1&amp;frs=1&amp;content_source=1fc82e51759cd729859b13944268283526c45c7f%253A1773370947</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>(770)</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/53277887/c/1587/1587/292/377/il/7142df/6463600074/il_340x270.6463600074_2mu1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Elegant Galaxy Healing Oval Blue Sandstone Engagement Ring Moss Agate Wedding Ring Vintage 14k Rose Gold June Birthstone Alexandrite Ring</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>39.90</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1779023082/elegant-galaxy-healing-oval-blue?click_key=6f2407c618c62e49da8d680b5c0ad9c5d7ad0aa1%3A1779023082&amp;click_sum=4a1c517c&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-13&amp;pro=1&amp;frs=1</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>(664)</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/42136421/c/1388/1388/305/291/il/ccfaee/6316171943/il_340x270.6316171943_6sly.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>14k Gold Map of Israel pendant, Gold Israel Pendant, Eilat Stone Pendant, Gold Jewish Pendant, Map necklace pendant, Israel Jewelry</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>693.00</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1555786865/14k-gold-map-of-israel-pendant-gold?click_key=57134af2674895f93ad02c23d338ebe1876a04c3%3A1555786865&amp;click_sum=ca54dd83&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-14&amp;frs=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>(301)</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/23295999/r/il/e9cd0b/5300031785/il_340x270.5300031785_9ixt.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Vintage kite cut green moss agate engagement ring set 14k rose gold marquise cut diamond ring women unique bridal wedding ring set gift</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>131.20</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1777988101/vintage-kite-cut-green-moss-agate?click_key=0bb68d76aaa58edb68731fefe1d4ec08b2cbc59a%3A1777988101&amp;click_sum=be92dd33&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-15&amp;pro=1&amp;sts=1</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>(9,342)</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/14110719/c/1388/1103/35/124/il/ab380f/3712342121/il_340x270.3712342121_fl43.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Nature Inspired Bee,Fox and Dinosaur Claws Engagement Ring w/ Oval Cut Montana Sapphire,Teal Sapphire engagement Ring,Unique Engagement Ring</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>3,600.00</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4307727574/nature-inspired-beefox-and-dinosaur?click_key=07094de73745d9b87a7ff54272b9287b1eb77acd%3A4307727574&amp;click_sum=562446c8&amp;ls=a&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165450-1-16</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>(81)</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/22798206/r/il/ebf158/6921723911/il_340x270.6921723911_38pk.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>In Box CH Silver Punk cross bracelet gothic style Jewelry cross rosary letter chain Birthday Gift</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>32.98</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4299184491/in-box-ch-silver-punk-cross-bracelet?click_key=ecb3f040d9cf2b8aa628f71b8fa5586238edcffa%3A4299184491&amp;click_sum=20c2ff45&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-37&amp;pro=1&amp;content_source=ecb3f040d9cf2b8aa628f71b8fa5586238edcffa%253A4299184491</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>(6)</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/58053909/r/il/7833b0/6830614112/il_340x270.6830614112_909z.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>CH In Box 925 Silver Cemetery zircon Cross silver rings Dagger ring man woman neutral couple Ring punk y2k opium Gothic designer jewelry</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>31.56</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/4304973761/ch-in-box-925-silver-cemetery-zircon?click_key=e1f6bf0c011cf74f2b625c315adcc8d94ae51ee1%3A4304973761&amp;click_sum=61a1f4cb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-38&amp;pro=1&amp;frs=1&amp;content_source=e1f6bf0c011cf74f2b625c315adcc8d94ae51ee1%253A4304973761</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>(1)</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/53924353/r/il/ac36c6/6859717574/il_340x270.6859717574_gto1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Crystal Sun and Moon Earrings, Dangle Earrings, Wire Wrap Crystal Earrings</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>15.78</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1295706184/crystal-sun-and-moon-earrings-dangle?click_key=67706e6917ce1bd62369d6c567fef4927822077c%3A1295706184&amp;click_sum=3f0cb329&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-39&amp;pro=1&amp;sts=1&amp;content_source=67706e6917ce1bd62369d6c567fef4927822077c%253A1295706184</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>(1,177)</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/27245498/r/il/5f4a6f/4237309847/il_340x270.4237309847_jnm5.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Mystery Jewelry Jars, Vintage Style Mystery Jewelry Jar, Mystery Jewelry Lot of Necklaces Pendants Bracelets Rings Earrings, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>14.57</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1882002443/mystery-jewelry-jars-vintage-style?click_key=336bea60fe608e31b326b31ff39be42d4ff05b3f%3A1882002443&amp;click_sum=a602eeec&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-40&amp;pro=1&amp;content_source=336bea60fe608e31b326b31ff39be42d4ff05b3f%253A1882002443</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>(165)</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/55418552/r/il/101a03/6851948095/il_340x270.6851948095_ha47.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Gold Earrings, Gold Disc Earrings, Silver Earrings, Circle Earrings, Handmade Jewelry, Gold Jewelry Gift, Round Earrings, Gold Stud Earrings</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>37.29</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1128664829/gold-earrings-gold-disc-earrings-silver?click_key=3d39b0ec2628066f0b852035d08b2468553050a0%3A1128664829&amp;click_sum=e338fe92&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-41&amp;etp=1&amp;sts=1&amp;content_source=3d39b0ec2628066f0b852035d08b2468553050a0%253A1128664829</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>(3,514)</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/17763464/c/1626/1292/55/291/il/860a78/3543836963/il_340x270.3543836963_ebw0.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Leather travel jewelry case,Leather jewelry storage,Personalized jewelry organizer,Leather jewelry roll,Personalized jewelry roll</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>48.60</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1376195359/leather-travel-jewelry-caseleather?click_key=90f51fc190850b61be0b632faed0a4b2473c8da1%3A1376195359&amp;click_sum=97c6e4e5&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-42&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=90f51fc190850b61be0b632faed0a4b2473c8da1%253A1376195359</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>(1,890)</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/19642071/r/il/cd4ad6/4451985490/il_340x270.4451985490_blz6.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Against the Current Sterling Silver Ring | Adjustable Blue Fish Ring for Men &amp; Women | Unique Swimming Fish Design | Symbolic Jewelry Gift</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>33.72</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1854693866/against-the-current-sterling-silver-ring?click_key=c001347597cbc3d7c78d37640dd273902b4ff8fa%3A1854693866&amp;click_sum=afab10c7&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-43&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=c001347597cbc3d7c78d37640dd273902b4ff8fa%253A1854693866</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>(31)</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/56974458/r/il/63d1fd/6617860330/il_340x270.6617860330_kz7v.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Forget-Me-Not Necklace, Necklace for Women, Real Pressed Flower Jewerly, Forgetmenot, Flower Resin Jewelry, Bridesmaid Gifts, Gift for Her</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>18.69</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1774008366/forget-me-not-necklace-necklace-for?click_key=7abf4adb1f4ec8f9b2c6b3c48e7f16cd0944ec5f%3A1774008366&amp;click_sum=61eafc36&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-44&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=7abf4adb1f4ec8f9b2c6b3c48e7f16cd0944ec5f%253A1774008366</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>(1,928)</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/50890964/r/il/b7f1ae/6244433320/il_340x270.6244433320_4cf4.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Billie Eilish Blohsh Inspired Pendant Stainless Steel And Alloy Necklace</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>15.30</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1898349213/billie-eilish-blohsh-inspired-pendant?click_key=348ebec74056be580e56b2df724559907c14bfd3%3A1898349213&amp;click_sum=0e6ef5cb&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-45&amp;pro=1&amp;content_source=348ebec74056be580e56b2df724559907c14bfd3%253A1898349213</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>(26)</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/50765934/r/il/daedea/6791549852/il_340x270.6791549852_mggb.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Italian Bracelet,Custom silver Italy Charms,Personalized Italian Bracelet,Vintage Jewelry Gifts for Her,Birthday gift,Christmas gift</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>20.35</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1863639536/italian-braceletcustom-silver-italy?click_key=6b62e87dd9c51189ff12f1bd812a1b52cabc826e%3A1863639536&amp;click_sum=0424af10&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-46&amp;pro=1&amp;sts=1&amp;content_source=6b62e87dd9c51189ff12f1bd812a1b52cabc826e%253A1863639536</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>(51)</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/35651222/r/il/24c105/6710768929/il_340x270.6710768929_jvfd.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Pandora Beaded Bracelet, European Charm Bracelets, S925 sterling silver heart clasp snake chain bracelet, Birthday gift for girlfriend</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>28.99</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1879251072/pandora-beaded-bracelet-european-charm?click_key=07fbbf24ff8a8f4a33f30183487af5dcb259a6e8%3A1879251072&amp;click_sum=eec55a06&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-47&amp;pro=1&amp;content_source=07fbbf24ff8a8f4a33f30183487af5dcb259a6e8%253A1879251072</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>(62)</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/51978889/r/il/d9d88f/6742749410/il_340x270.6742749410_6gt5.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>If Friends were Flowers I'd Pick You Ring Dish,Personalized Birth Flower Jewelry Dish,Floral Trinket Dish for Friend,Birthday Gift for BFF</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>8.95</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1813761409/if-friends-were-flowers-id-pick-you-ring?click_key=a37ca940f7d23bd5ebd174bc7bdc440bfadf7c2b%3A1813761409&amp;click_sum=01da85b6&amp;ls=s&amp;ga_order=most_relevant&amp;ga_search_type=all&amp;ga_view_type=gallery&amp;ga_search_query=&amp;ref=search_grid-165451-1-48&amp;pro=1&amp;frs=1&amp;sts=1&amp;content_source=a37ca940f7d23bd5ebd174bc7bdc440bfadf7c2b%253A1813761409</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>(2,634)</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>https://i.etsystatic.com/48621519/c/1785/1785/107/81/il/a655af/6417461479/il_340x270.6417461479_pi4e.jpg</t>
         </is>
       </c>
     </row>
@@ -2244,22 +3972,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalized Name Necklace by Caitlyn Minimalist • Delicate Layering Necklace • Dainty Name Charm Jewelry • Mothers Day Gift • NM03F106 by CaitlynMinimalist</t>
+          <t>Mother of Pearl Tulip Necklace by Caitlyn Minimalist • Vintage Style Flower Pendant Necklace • Dainty Jewelry • Gifts for Mom • NR249 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1551096207/personalized-name-necklace-by-caitlyn?ref=rss</t>
+          <t>https://www.etsy.com/listing/1833440961/mother-of-pearl-tulip-necklace-by?ref=rss</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:11:28 -0400</t>
+          <t>Mon, 19 May 2025 16:01:26 -0400</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/e6b2b0/5403812830/il_570xN.5403812830_ar3l.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;37.00 USD&lt;/p&gt;&lt;p class="description"&gt;D A I N T Y ∙ N A M E ∙ N E C K L A C E&lt;br /&gt;&lt;br /&gt;Discover our Dainty Personalized Name Necklace, a truly one-of-a-kind piece. It's the perfect gift, whether it's for yourself or your special someone!&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Dimensions: Depending on your font choice, height sizes range from 3mm to 4mm lowercase.&lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold &lt;br /&gt;&lt;br /&gt;♡ Model showcases a fashionable layering look featuring: &lt;br /&gt;• Dainty Mirror Chain: https://etsy.me/3RnmrAr&lt;br /&gt;• Pave Linked Pendant Necklace: https://etsy.me/47yBwET&lt;br /&gt;• Birthstone Hoop Earrings: https://etsy.me/48ivLf6&lt;br /&gt;&lt;br /&gt;• All our jewelry is custom made by hand with Love and Care in our workshop ♡&lt;br /&gt;&lt;br /&gt;H O W ∙ T O ∙ O R D E R &lt;br /&gt;&lt;br /&gt;• Simply use the 'PERSONALIZATION BOX' to let us know the NAME and the FONT NUMBER that you would like. (Any font is available, not just our featured fonts)&lt;br /&gt;&lt;br /&gt;♡ NAME + FONT NUMBER ♡&lt;br /&gt;&lt;br /&gt;• Your piece will be created in Featured Font #106 if a font isn’t specified.&lt;br /&gt;&lt;br /&gt;• Birthstone Add-on: More ways to personalize your Necklace with our Dainty Birthstone Charm for $10 using this listing: &lt;br /&gt;&lt;br /&gt;http://etsy.me/2tqNhh5&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• The length option is the TOTAL length (including the charm). If you order a 18&amp;quot; chain, the piece will come as CHAIN + CHARM = 18&amp;quot;. All pieces come with a 1&amp;quot; extension chain so you can FINE TUNE the fit.&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready To Gift in elegant, reusable and recyclable jewelry boxes ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is custom made to order. Our turn around time is about 6 - 9 business days. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/912fe6/6531894949/il_570xN.6531894949_8yf8.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;42.00 USD&lt;/p&gt;&lt;p class="description"&gt;P E A R L ∙ T U L I P ∙ N E C K L A C E &lt;br /&gt;&lt;br /&gt;Celebrate grace and renewal with our Mother of Pearl Tulip Necklace, an homage to nature’s elegance. Featuring a delicate Tulip flower framed against a Mother of Pearl backdrop, this piece captures the soft beauty of blooming petals. Perfect for adding a touch of timeless charm to your jewelry collection ♡ &lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver&lt;br /&gt;&lt;br /&gt;• Finish: 18K Gold ∙ Sterling Silver &lt;br /&gt;&lt;br /&gt;• Featuring a ~10x12mm Mother of Pearl Tulip Pendant on a dainty Cable Chain, adjustable from 16 to 18 inches.&lt;br /&gt;&lt;br /&gt;♡ Model showcases a diverse, eclectic look featuring: &lt;br /&gt;• Duo Chain Necklace: https://etsy.me/49lZeFV&lt;br /&gt;• Pearl Signet Ring: https://etsy.me/3AtOYhX&lt;br /&gt;• Beaded Ring: https://etsy.me/4bzq24U&lt;br /&gt;• Chunky Statement Ring: https://etsy.me/3KU4jcU&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times.&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S &lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;---------------------------------------------- &lt;br /&gt; +• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2271,22 +4000,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Agate Earring Set by Caitlyn Minimalist • Green Gemstone Dangle Earring, Stud Earring, &amp; Huggie Hoop with Charm • Best Friend Gift • ER437 by CaitlynMinimalist</t>
+          <t>Initial Heart Locket Necklace by Caitlyn Minimalist • Gold Locket Photo Necklace with Twist Chain • Personalized Gift for Mom • NR108 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1668754028/agate-earring-set-by-caitlyn-minimalist?ref=rss</t>
+          <t>https://www.etsy.com/listing/1380857815/initial-heart-locket-necklace-by-caitlyn?ref=rss</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:07:43 -0400</t>
+          <t>Mon, 19 May 2025 15:54:28 -0400</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/aa0202/5842766663/il_570xN.5842766663_sjlf.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;46.50 USD&lt;/p&gt;&lt;p class="description"&gt;A G A T E ∙ E A R R I N G ∙ S E T&lt;br /&gt;&lt;br /&gt;Three single earrings work harmoniously together in our Agate Earring Set. The unique swirled green design of the Agate stone creates a new look every time you wear them. With a hoop earring, stud earring, and a drop earring you can wear them all together or split them between your ears. No matter what, you’ll always have a unique look to show off.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: 18K Gold ∙ Sterling Silver &lt;br /&gt;&lt;br /&gt;• Featuring a Set of 3 Agate CZ Gemstone Earrings (Agate May Vary in Color): &lt;br /&gt;1) ~4mm Dangling Agate Pave Huggie Hoop: ~8mm Inner Diameter | ~12mm Outer Diameter&lt;br /&gt;2) ~6mm Agate Stud Earring&lt;br /&gt;3) ~12mm Agate Diamond Drop Stud Earring &lt;br /&gt;&lt;br /&gt;♡♡ This listing can be purchased as a Set of 3 Single Earrings or as a Full Set of 3 Earring Pairs (Save 10%). You may choose the option you'd like in the drop down menu ♡♡ &lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡ &lt;br /&gt;&lt;br /&gt;• Gift wrapping with ribbon is available at check out. Ordering multiple pieces? Leave a note at checkout and we'll discreetly label each box with its name.&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;br /&gt;&lt;br /&gt;• SKU: BB-EB011&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/c899dd/4514803139/il_570xN.4514803139_bw2m.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;42.00 USD&lt;/p&gt;&lt;p class="description"&gt;I N I T I A L ∙ H E A R T ∙ L O C K E T&lt;br /&gt;&lt;br /&gt;Immortalize your story with our Initial Heart Locket 🤍 The heart-shaped locket can be personalized with an engraved initial, and hold your favorite photo and treasured mementos. The pendant is complemented by a Singapore twist chain for a touch of sparkle. This keepsake makes for a special gift for Valentine's Day, Mother's Day, Anniversaries or any significant occasion.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver&lt;br /&gt;&lt;br /&gt;• Finish: 18K Gold&lt;br /&gt;&lt;br /&gt;• Featuring ~12 x 12.5mm Pendant  |  ~7.2mm Inner Photo Size  |  Adjustable Singapore Twist Chain from 16&amp;quot; to 18&amp;quot;&lt;br /&gt;&lt;br /&gt;♡ Please note: Locket comes without a photo. Photo insertion services are not included ♡&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡ &lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2298,22 +4027,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Trinity Knot Earrings by Caitlyn Minimalist • Dainty Mixed Metal Stud Earrings • Minimalist Jewelry • Perfect Anniversary Gift • ER286 by CaitlynMinimalist</t>
+          <t>Rope Chain Necklace in Gold, Rose Gold, Sterling Silver by Caitlyn Minimalist • Thick Necklace • Men Necklace • Perfect Gift for Him • NR023 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1303577181/trinity-knot-earrings-by-caitlyn?ref=rss</t>
+          <t>https://www.etsy.com/listing/875715598/rope-chain-necklace-in-gold-rose-gold?ref=rss</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:06:33 -0400</t>
+          <t>Mon, 19 May 2025 15:52:31 -0400</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/d1b18f/4340208167/il_570xN.4340208167_dcj1.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;23.50 USD&lt;/p&gt;&lt;p class="description"&gt;T R I N I T Y ∙ K N O T ∙ E A R R I N G S&lt;br /&gt;&lt;br /&gt;Dainty and minimalist, these handmade love knot studs are the perfect way to celebrate a milestone anniversary. The three-knot motif is known as a trinity knot, which symbolizes love, luck and faithfulness. A symbol fit for the brilliant person in your life that means something special to you both.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold&lt;br /&gt;&lt;br /&gt;• Featuring ~7.5mm Tri-Color Knot Stud Earrings | Sold as a Pair&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged ready to gift in elegant jewelry boxes. &lt;br /&gt;&lt;br /&gt;• If you can't find the information you need or need some advice for your design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will ship separated into two shipments. Our turn around time is about 6 - 10 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;O U R ∙ P O L I C I E S&lt;br /&gt;http://etsy.me/2cuqINv&lt;br /&gt;&lt;br /&gt;A B O U T ∙ C A I T L Y N M I N I M A L I S T ♡&lt;br /&gt;http://etsy.me/2cYBUSp&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;I N S I D E ∙ S C O O P&lt;br /&gt;• IG: @CaitlynMinimalist&lt;br /&gt;• FB: https://www.facebook.com/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;-----------------------♡--------------------&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt; Kate &lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;•  All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/3ea482/2601187240/il_570xN.2601187240_la6g.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;42.00 USD&lt;/p&gt;&lt;p class="description"&gt;R O P E ∙ C H A I N ∙ N E C K L A C E &lt;br /&gt;&lt;br /&gt;Our Rope Chain Necklace, as its name suggests, is linked in a twisted pattern to resemble a rope. This timeless, layering piece is a simple and understated way to bring elegance to any ensemble. Add instant sparkle to your look, while never overpowering your clothing with this statement jewelry choice.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold&lt;br /&gt;&lt;br /&gt;• Featuring 1.5mm Rope Chain, adjustable length 16 inches to 18 inches.&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged ready to gift in elegant jewelry boxes. &lt;br /&gt;&lt;br /&gt;• If you can't find the information you need or need some advice for your design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will ship separated into two shipments. Our turn around time is about 6 - 10 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;O U R ∙ P O L I C I E S&lt;br /&gt;http://etsy.me/2cuqINv&lt;br /&gt;&lt;br /&gt;A B O U T ∙ C A I T L Y N M I N I M A L I S T ♡&lt;br /&gt;http://etsy.me/2cYBUSp&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;I N S I D E ∙ S C O O P&lt;br /&gt;• IG: @CaitlynMinimalist&lt;br /&gt;• FB: https://www.facebook.com/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2325,22 +4054,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ball Stud Earrings by Caitlyn Minimalist • Double Sphere Earrings • Minimalist Earrings • Dainty Gold Earrings • Gift for Her • ER130 by CaitlynMinimalist</t>
+          <t>Heart Carabiner Charm Set by Caitlyn Minimalist • Set of 2: Heart Clasp Charms for Bracelet &amp; Necklace • Gold Jewelry • Gift for Her • XR043 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1006418643/ball-stud-earrings-by-caitlyn-minimalist?ref=rss</t>
+          <t>https://www.etsy.com/listing/4304327002/heart-carabiner-charm-set-by-caitlyn?ref=rss</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:03:03 -0400</t>
+          <t>Mon, 19 May 2025 15:49:17 -0400</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/069a8e/3110476322/il_570xN.3110476322_3v46.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;26.50 USD&lt;/p&gt;&lt;p class="description"&gt;B A L L ∙ S T U D ∙ E A R R I N G S&lt;br /&gt;&lt;br /&gt;Simple and versatile, the Ball Studs are the perfect starter earrings for those who are just dipping their toes into stacked jewelry. We have taken the classic ball stud earrings and modernized it with a screw-on ball backing for more security. Put these on and forget about them, since they go with every outfit anyway.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold&lt;br /&gt;&lt;br /&gt;• Featuring ~5mm Minimal Duo Ball Studs&lt;br /&gt;&lt;br /&gt;• Sold as a pair&lt;br /&gt;&lt;br /&gt;F L A T B A C K · S T U D S · G U I D E&lt;br /&gt;&lt;br /&gt;Our flatback earrings or nap earrings are an easy and comfortable choice when it comes to wearing earrings for long periods of time. &lt;br /&gt;&lt;br /&gt;Here is a simple guide for wearing your flatback earrings:&lt;br /&gt;&lt;br /&gt;1. SEPARATE: Screw off the front of the stud earring.&lt;br /&gt;     •  TIP! Flat back earrings will have the post attached to the back of the earring.&lt;br /&gt;2. INSERT STUD: Push the backing of the earring in first. While keeping it in place, gently screw on the front of the earring.&lt;br /&gt;3. REMOVAL: Keeping the back of the earring in place, gently unscrew the front piece and pull it away from the earring.&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged ready to gift in elegant jewelry boxes. Our jewelry boxes are reusable and recyclable ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;O U R ∙ P O L I C I E S&lt;br /&gt;http://etsy.me/2cuqINv&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/fbb41f/6859360488/il_570xN.6859360488_cbd4.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;39.00 USD&lt;/p&gt;&lt;p class="description"&gt;H E A R T ∙ C A R A B I N E R ∙ C H A R M S&lt;br /&gt;&lt;br /&gt;Add a heartfelt twist to your jewelry styling with our Heart Carabiner Charm Set ♡ Featuring two heart-shaped carabiners—one with a smooth polished finish and one with a bold rope texture—this set offers the perfect blend of charm and versatility. Use them as connectors for charm bracelets, necklaces, or keychains to create a look that’s all your own!&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: 18K Gold ∙ Sterling Silver &lt;br /&gt;&lt;br /&gt;• Featuring a Set of 2 Carabiner Clasp Charms:&lt;br /&gt;1) ~12x16mm Heart Carabiner&lt;br /&gt;2) ~13x16mm Ribbed Heart Carabiner&lt;br /&gt;&lt;br /&gt;♡ Model showcases a chic, personalized layering look featuring:&lt;br /&gt;• Duo Knot Earrings: https://etsy.me/4j0kjZy&lt;br /&gt;• Link Strap Necklace: https://etsy.me/3SzekQF&lt;br /&gt;• Diamond Link Necklace: https://etsy.me/3W5cvfW&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡ &lt;br /&gt;&lt;br /&gt;• Gift wrapping with ribbon is available at check out. Ordering multiple pieces? Leave us a note and we'll discreetly label each box with the item's name.&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2352,22 +4081,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Family Necklace • Personalized Gift • Linked Circle Necklace •  Custom Children Name Rings • Eternity Necklace • Mother Gift • NM30F30 by CaitlynMinimalist</t>
+          <t>Huggie Earrings by Caitlyn Minimalist • Huggie Hoop Earrings in Gold, Sterling Silver, Rose Gold • Perfect For Everyday Wear • ER007 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/492227219/family-necklace-personalized-gift-linked?ref=rss</t>
+          <t>https://www.etsy.com/listing/868385833/huggie-earrings-by-caitlyn-minimalist?ref=rss</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:03:01 -0400</t>
+          <t>Mon, 19 May 2025 15:48:01 -0400</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/fb2b79/1130332425/il_570xN.1130332425_rvw1.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;42.00 USD&lt;/p&gt;&lt;p class="description"&gt;E T E R N I T Y ∙ N E C K L A C E&lt;br /&gt;&lt;br /&gt;Celebrate the bonds of family with our exquisite Family Necklace. This personalized linked circle necklace features custom children name rings, symbolizing the unbreakable connection and love between family members. Crafted with care, this eternity necklace is a meaningful and elegant piece, perfect as a mother gift or a thoughtful personalized gift for any occasion.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Dimension: 13mm Outer Diameter&lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold&lt;br /&gt;&lt;br /&gt;• Personalized: This design can be customized with your Roman Numerals, Messages, Coordinates or Names.&lt;br /&gt;&lt;br /&gt;• All our work is custom made by hand with Love and Care in our workshop ♡&lt;br /&gt;&lt;br /&gt;H O W ∙ T O ∙ O R D E R &lt;br /&gt;&lt;br /&gt;• Simply use the 'PERSONALIZATION BOX' upon ordering to let us know the ROMAN NUMERALS/MESSAGES/LETTERS and FONT that you would like using this format: &lt;br /&gt; &lt;br /&gt;-- CHAIN COLOR: &lt;br /&gt;&lt;br /&gt;-- CIRCLE 1: (Material type &amp; Engraving) &lt;br /&gt;&lt;br /&gt;-- CIRCLE 2: (Material type &amp; Engraving) &lt;br /&gt;&lt;br /&gt;-- CIRCLE 3: (Material type &amp; Engraving) &lt;br /&gt;&lt;br /&gt;-- FONT NUMBER:&lt;br /&gt;&lt;br /&gt;• Design can be personalized with up to 8 circles for an additional $5 per circle. &lt;br /&gt;&lt;br /&gt;• Listing necklace features font #30. If a font is not given, you will receive the font that is pictured.&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is custom made to order. Our turn around time is about 6 - 9 business days. This can change during peak seasons. Please check our home page for the most current times.&lt;br /&gt;&lt;br /&gt;• Expedited shipping is available during check out. It will speed up the transit time, but does not change our production time (see above).&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/b1dc1d/2518543302/il_570xN.2518543302_l6du.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;20.50 USD&lt;/p&gt;&lt;p class="description"&gt;H U G G I E ∙ H O O P S&lt;br /&gt;&lt;br /&gt;Our Huggie Earrings are a customer favorite for a reason. With their classic, versatile design, they pair perfectly with any look, making them a top choice for everyday wear.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold&lt;br /&gt;&lt;br /&gt;• Dimensions: Inner Diameter: ~6mm | Outer Diameter: ~10mm. &lt;br /&gt;&lt;br /&gt;• Featuring Editor Huggie Hoops, Ultra Light Weight Design. Wear these all day, every day and forget they’re even on your ear | Sold as a Pair &lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡ &lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2379,22 +4108,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Perfect Gift for Her • Minimalist Name Necklace by CaitlynMinimalist in Sterling Silver, Gold and Rose Gold • Accessories for Mom • NH02F66 by CaitlynMinimalist</t>
+          <t>Pink Velvet Heart Ring Box by Caitlyn Minimalist • Ring Storage Case with Ribbon • Coquette Gift Boxes • Romantic Anniversary Gift • XR025 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/742468036/perfect-gift-for-her-minimalist-name?ref=rss</t>
+          <t>https://www.etsy.com/listing/1745333681/pink-velvet-heart-ring-box-by-caitlyn?ref=rss</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:02:33 -0400</t>
+          <t>Mon, 19 May 2025 15:46:47 -0400</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/5edd71/2145834607/il_570xN.2145834607_2vz6.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;37.00 USD&lt;/p&gt;&lt;p class="description"&gt;D A I N T Y ∙ N A M E ∙ N E C K L A C E&lt;br /&gt;&lt;br /&gt;Create a custom necklace that embodies simplicity and grace with the Minimalist Name Necklace. Available in sterling silver, gold, and rose gold, this elegant necklace features a sleek and stylish design that adds a touch of personal charm to any outfit. &lt;br /&gt;&lt;br /&gt;Its minimalist design ensures it complements any style, making it a versatile addition to her jewelry collection. Celebrate the special moments and show your appreciation with a personalized piece that speaks from the heart.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Dimensions: Depending on your font choice, height sizes range from 3mm to 4mm lowercase.&lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold &lt;br /&gt;&lt;br /&gt;• All our jewelry is custom made by hand with Love and Care in our workshop ♡&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;H O W ∙ T O ∙ O R D E R &lt;br /&gt;&lt;br /&gt;• Simply use the 'PERSONALIZATION BOX' to let us know the NAME and the FONT NUMBER that you would like. (Any font is available, not just our featured fonts)&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;♡ NAME + FONT NUMBER ♡&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;• Listing necklace features FONT #66. If a font is not given, you will receive the font that is pictured.&lt;br /&gt;&lt;br /&gt;• Birthstone Add-on: More ways to personalize your Necklace with our Dainty Birthstone Charm for $10 using this listing: &lt;br /&gt;&lt;br /&gt;http://etsy.me/2tqNhh5&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• The length option is the TOTAL chain length (including the charm). If you order an 18&amp;quot; chain, the piece will come as CHAIN + CHARM = 18&amp;quot;. All pieces will come with a 1&amp;quot; extension chain so you can FINE TUNE the fit.&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged ready to gift in elegant jewelry boxes. &lt;br /&gt;&lt;br /&gt;• If you can't find the information you need or need some advice for your design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• All items are custom made to order. Our turn around time is about 6 - 10 business days. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;• Rush your order: Please contact us to see if we can meet your deadline. You can also expedite your shipping in the drop down menu upon check out. This does not change production times (see above) &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;O U R ∙ P O L I C I E S&lt;br /&gt;http://etsy.me/2cuqINv&lt;br /&gt;&lt;br /&gt;A B O U T ∙ C A I T L Y N M I N I M A L I S T ♡&lt;br /&gt;http://etsy.me/2cYBUSp&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Custom Name NECKLACE ► http://etsy.me/2wDKySo&lt;br /&gt;&lt;br /&gt;I N S I D E ∙ S C O O P&lt;br /&gt;• IG: @CaitlynMinimalist&lt;br /&gt;• FB: https://www.facebook.com/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/a638b1/6098931785/il_570xN.6098931785_343w.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;16.00 USD&lt;/p&gt;&lt;p class="description"&gt;H E A R T ∙ V E L V E T ∙ R I N G ∙ B O X&lt;br /&gt;&lt;br /&gt;Love is in the air! Give someone you love something special in our Pink Velvet Heart Box. Soft and dreamy with a coquette style, this jewelry case can hold up to two rings. Finishing with a delicate pink bow to tie around the ring box, you will have a gift that is set and ready to give.&lt;br /&gt;&lt;br /&gt;• Made of soft Pink Velvet &lt;br /&gt;&lt;br /&gt;• Featuring a Two Slot, ~2x2x1.5 inch Velvet Heart Jewelry Box with a ~14 inch Pink Ribbon.&lt;br /&gt;&lt;br /&gt;• Our Ring Case is compact enough to fit in your luggage wherever you go while still keeping your jewelry in place. &lt;br /&gt;&lt;br /&gt;• If you can't find the information you need or need some advice for your design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will ship separated into two shipments. Our turn around time is about 6 - 10 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;O U R ∙ P O L I C I E S&lt;br /&gt;http://etsy.me/2cuqINv&lt;br /&gt;&lt;br /&gt;A B O U T ∙ C A I T L Y N M I N I M A L I S T ♡&lt;br /&gt;http://etsy.me/2cYBUSp&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;I N S I D E ∙ S C O O P&lt;br /&gt;• IG: @CaitlynMinimalist&lt;br /&gt;• FB: https://www.facebook.com/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;-----------------------♡--------------------&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt; Kate &lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2406,22 +4135,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Custom Baguette Gemstone Ring by Caitlyn Minimalist • Personalized Statement Ring • Mothers Ring with Birthstones • Baby Shower Gift • RM106 by CaitlynMinimalist</t>
+          <t>Reusable Ring Sizer • Adjustable, US Ring Size Tool Full &amp; Half Sizes • Find Your Accurate Ring Size • Easy to Use Finger Measurer • RX010 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1454235998/custom-baguette-gemstone-ring-by-caitlyn?ref=rss</t>
+          <t>https://www.etsy.com/listing/1075563860/reusable-ring-sizer-adjustable-us-ring?ref=rss</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:00:19 -0400</t>
+          <t>Mon, 19 May 2025 15:46:47 -0400</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/a8fee5/4979155735/il_570xN.4979155735_qekx.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;33.00 USD&lt;/p&gt;&lt;p class="description"&gt;B A G U E T T E ∙ S T O N E ∙ R I N G &lt;br /&gt;&lt;br /&gt;This personalized statement ring features beautiful baguette stones that can be customized with your choice of birthstones. Whether you're looking for a meaningful Mother's ring with birthstones representing your loved ones, or a special baby shower gift for a mom-to-be, this ring is sure to impress.&lt;br /&gt;&lt;br /&gt;♡ This listing is just for one ring ♡ If you would like a set of rings, simply change the quantity as you wish upon check out ♡&lt;br /&gt; &lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver,  &lt;br /&gt;&lt;br /&gt;• Stone Dimensions: ~5mm x 2mm CZ Baguettes&lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold &lt;br /&gt;&lt;br /&gt;• All our work is custom made by hand with Love and Care in our workshop ♡&lt;br /&gt;&lt;br /&gt;H O W ∙ T O ∙ O R D E R &lt;br /&gt;&lt;br /&gt;• Simply use the 'PERSONALIZATION BOX' upon ordering to let us know the BIRTHSTONE(S) you would like.&lt;br /&gt; &lt;br /&gt;♡ YOUR BIRTHSTONE(S) ♡&lt;br /&gt;&lt;br /&gt;• Design can be personalized with the following BIRTHSTONE COLORS:&lt;br /&gt;&lt;br /&gt;January - Garnet&lt;br /&gt;February - Amethyst&lt;br /&gt;March - Aquamarine&lt;br /&gt;April - Clear Crystal&lt;br /&gt;May - Emerald&lt;br /&gt;June - Alexandrite&lt;br /&gt;July - Pink Ruby&lt;br /&gt;August - Dark Peridot&lt;br /&gt;September - Sapphire&lt;br /&gt;October - Light Tourmaline&lt;br /&gt;November - Yellow Topaz&lt;br /&gt;December - Blue Zircon&lt;br /&gt;Opal&lt;br /&gt;Black CZ Diamond &lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is custom made to order. Our turn around time is about 6 - 9 business days. This can change during peak seasons. Please check our home page for the most current times.&lt;br /&gt;&lt;br /&gt;• Expedited shipping is available during check out. It will speed up the transit time, but does not change our production time (see above).&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/75cb80/3349594256/il_570xN.3349594256_jm9w.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;1.20 USD&lt;/p&gt;&lt;p class="description"&gt;A D J U S T A B L E • U S • R I N G • S I Z E R&lt;br /&gt;&lt;br /&gt;Discover your ideal ring size on-the-spot with this super-handy adjustable reusable ring sizer. It’s made from soft, flexible plastic and can be used over and over again so there’s no need to worry about trying on rings in store or relying on paper or string. Adjustable to fit any finger, this ring sizer lets you find the perfect fit using our unique sliding system – just slide it on and the gauge will work its magic by showing off your true size.&lt;br /&gt;&lt;br /&gt;• Made of soft flexible plastic in black with gold foil numbers. &lt;br /&gt;&lt;br /&gt;• Adjustable, reusable, easy to use and very handy to have around. &lt;br /&gt;&lt;br /&gt;• Measures US ring size from 1 - 17 in full and half sizes.&lt;br /&gt;&lt;br /&gt;• If you can't find the information you need or need some advice for your design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will ship separated into two shipments. Our turn around time is about 6 - 10 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;O U R ∙ P O L I C I E S&lt;br /&gt;http://etsy.me/2cuqINv&lt;br /&gt;&lt;br /&gt;A B O U T ∙ C A I T L Y N M I N I M A L I S T ♡&lt;br /&gt;http://etsy.me/2cYBUSp&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;I N S I D E ∙ S C O O P&lt;br /&gt;• IG: @CaitlynMinimalist&lt;br /&gt;• FB: https://www.facebook.com/CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;-----------------------♡--------------------&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt; Kate &lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2433,22 +4162,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Triple Marquise Birthstone Ring Caitlyn Minimalist • Dainty Custom Gemstone Ring • Personalized Jewelry • Accessories for Mom • RM120 by CaitlynMinimalist</t>
+          <t>Dainty Engraved Flower Ring by CaitlynMinimalist • Personalized Stackable Ring • Custom Friendship Ring • Gifts for Mom • RM21 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1631920332/triple-marquise-birthstone-ring-caitlyn?ref=rss</t>
+          <t>https://www.etsy.com/listing/1215408499/dainty-engraved-flower-ring-by?ref=rss</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:59:08 -0400</t>
+          <t>Mon, 19 May 2025 15:44:42 -0400</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/cc5117/5665557800/il_570xN.5665557800_1wi0.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;35.00 USD&lt;/p&gt;&lt;p class="description"&gt;M A R Q U I S E ∙ B I R T H S T O N E ∙ R I N G &lt;br /&gt;&lt;br /&gt;Your ultimate stacking ring has arrived! Our Triple Marquise Birthstone Ring allows you to customize to the stone you want. With delicate CZ Diamond gemstones in between each marquise birthstone, this ring shines with even more sparkle.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold &lt;br /&gt;&lt;br /&gt;• Featuring a ~1mm Dainty Ring Band with three ~3.5 x 2mm Marquise Gemstones and ~1mm Round CZ Diamond Stones.&lt;br /&gt;&lt;br /&gt;♡ Model showcases a beautiful, iridescent ring stack featuring:&lt;br /&gt;• Opal Inlay Ring: https://etsy.me/3RRxRfZ&lt;br /&gt;• Delicate Opal Ring: https://etsy.me/47qyscP&lt;br /&gt;• Thin Double Band Ring: https://etsy.me/4956zsN&lt;br /&gt;&lt;br /&gt;H O W ∙ T O ∙ O R D E R &lt;br /&gt;&lt;br /&gt;• Select your RING SIZE and BIRTHSTONE in the drop down menu. &lt;br /&gt;&lt;br /&gt;• Design can be personalized with the following BIRTHSTONE COLORS:&lt;br /&gt;&lt;br /&gt;January - Garnet&lt;br /&gt;February - Amethyst&lt;br /&gt;March - Aquamarine&lt;br /&gt;April - Clear Crystal&lt;br /&gt;May - Emerald&lt;br /&gt;June - Alexandrite&lt;br /&gt;July - Pink Ruby&lt;br /&gt;August - Peridot&lt;br /&gt;September - Sapphire&lt;br /&gt;October - Pink Tourmaline&lt;br /&gt;November - Topaz&lt;br /&gt;December - Blue Zircon&lt;br /&gt;Black CZ Diamond&lt;br /&gt;&lt;br /&gt;♡ ♡ The OPAL Marquise Ring in this listing can be found here: https://etsy.me/47qyscP ♡ ♡ &lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready To Gift in elegant, reusable and recyclable jewelry boxes ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is custom made to order. Our turnaround time is about 6 - 9 business days. This can change during peak seasons. Please check our home page for the most current times.&lt;br /&gt;&lt;br /&gt;• Expedited shipping is available during check out. It will speed up the transit time, but does not change our production time (see above).&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt; IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/f23573/3879475300/il_570xN.3879475300_kwxi.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;26.50 USD&lt;/p&gt;&lt;p class="description"&gt;D A I N T Y ∙ F L O W E R ∙ R I N G&lt;br /&gt;&lt;br /&gt;Embrace delicate beauty with our Personalizable Dainty Flower Ring – the perfect best friend gift or gift for her. Crafted with intricacy, this ring features a charming flower design that can be personalized to add a special touch. Symbolizing friendship and love, it's a timeless piece that celebrates the unique bond between friends or loved ones ♡ &lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Dimensions: 2.5mm Height&lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold ∙ Rose Gold &lt;br /&gt;&lt;br /&gt;• Personalization: Design can fit up to one flower design on both the inside and outside of the band. &lt;br /&gt;&lt;br /&gt;• All our work is custom made by hand with Love and Care in our workshop ♡&lt;br /&gt;&lt;br /&gt;H O W ∙ T O ∙ O R D E R &lt;br /&gt;&lt;br /&gt;• Simply use the 'PERSONALIZATION BOX' upon ordering to let us know the FLOWER you would like on the band.&lt;br /&gt;&lt;br /&gt;♡ YOUR FLOWER ♡&lt;br /&gt;&lt;br /&gt;• Messages can be engraved on two sides of the charm with an additional fee - $10. If you want an engraving on one side of the charm, choose ONE SIDED*. If you want engravings on both sides, choose DOUBLE SIDED*.&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This item is custom made to order. Our turn around time is about 6 - 9 business days. This can change during peak seasons. Please check our home page for the most current times.&lt;br /&gt;&lt;br /&gt;• Expedited shipping is available during check out. It will speed up the transit time, but does not change our production time (see above).&lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2460,22 +4189,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Starburst Huggie Earrings by Caitlyn Minimalist • Trending Opal Star Earrings • Perfect Minimalist Look • Jewelry Gift for Her • ER055 by CaitlynMinimalist</t>
+          <t>Dainty Pearl Stud Earrings by Caitlyn Minimalist • Everyday Pearl Jewelry • Minimalist Stacking Earrings • Bridesmaid Proposal Gifts • ER316 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/888157018/starburst-huggie-earrings-by-caitlyn?ref=rss</t>
+          <t>https://www.etsy.com/listing/1406358019/dainty-pearl-stud-earrings-by-caitlyn?ref=rss</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:59:06 -0400</t>
+          <t>Mon, 19 May 2025 15:41:16 -0400</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/c7b50b/2650731380/il_570xN.2650731380_87ln.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;33.00 USD&lt;/p&gt;&lt;p class="description"&gt;S T A R B U R S T ∙ H U G G I E ∙ E A R R I N G S&lt;br /&gt;&lt;br /&gt;The Starburst Huggies will bring an explosion of vibrance, light, and joy into your life! A luminescent opal stone is surrounded by sparkling pave diamonds that softly catch the light, for a star-studded appearance.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold&lt;br /&gt;&lt;br /&gt;• Hoop Dimensions: ~10mm Inner Diameter | ~13mm Outer Diameter&lt;br /&gt;&lt;br /&gt;• Featuring ~3mm Huggie Hoops with dangling ~5mm CZ Opal Starburst Charm | Sold as a Pair&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡ &lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/5668fb/4648000456/il_570xN.4648000456_3mmm.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;23.50 USD&lt;/p&gt;&lt;p class="description"&gt;P E A R L ∙ S T U D ∙ E A R R I N G S&lt;br /&gt;&lt;br /&gt;These delicate pearl stud earrings are easy to pair and stack with other pieces in your collection. Wear in the first piercing for a minimalist look or mix and match in multiple piercings to create your own unique set.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold &lt;br /&gt;&lt;br /&gt;• Featuring ~3.5mm Pearl Stud Earrings | Sold as a Pair&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged Ready to Gift in elegant, reusable and recyclable jewelry boxes ♡ &lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2487,22 +4216,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Dainty Diamond Necklace • Floating Diamond Solitaire Necklace • Minimalist Jewelry • Bridesmaid Necklace • Gift for Her • NR048 by CaitlynMinimalist</t>
+          <t>Diamond Climber Earrings by Caitlyn Minimalist • Tiny Diamond Stud Earrings • Dainty Jewelry for Everyday Wear • Mothers Day Gift • ER361 by CaitlynMinimalist</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1027340531/dainty-diamond-necklace-floating-diamond?ref=rss</t>
+          <t>https://www.etsy.com/listing/1522086991/diamond-climber-earrings-by-caitlyn?ref=rss</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:58:59 -0400</t>
+          <t>Mon, 19 May 2025 15:39:50 -0400</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/1d4562/3237332939/il_570xN.3237332939_tsfw.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;31.50 USD&lt;/p&gt;&lt;p class="description"&gt;D A I N T Y ∙ D I A M O N D ∙ N E C K L A C E &lt;br /&gt;&lt;br /&gt;With vintage inspiration, this dainty diamond necklace is minimalistic, yet bold enough to catch the eye. The circular shape and clear cz stone are so versatile they can take you from an important meeting to an exciting night out.&lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold &lt;br /&gt;&lt;br /&gt;• Featuring a 4mm Round CZ Diamond Charm with adjustable chain 16 inches to 18 inches. &lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged ready to gift in elegant jewelry boxes. Our jewelry boxes are reusable and recyclable ♡&lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :) &lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10204022/r/il/a2c1d2/5428800296/il_570xN.5428800296_7qag.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;26.50 USD&lt;/p&gt;&lt;p class="description"&gt;D I A M O N D ∙ C L I M B E R ∙ S T U D S&lt;br /&gt;&lt;br /&gt;Elevate your gifting game with our Diamond Climber Earrings, the perfect choice for celebrating special moments. These petite and elegant earrings, adorned with four subtly varying diamond stones, beautifully ascend your ear, making them a delightful and versatile gift for anniversaries, birthdays, or the holiday season ♡ &lt;br /&gt;&lt;br /&gt;• Material: High Quality Solid 925 Sterling Silver &lt;br /&gt;&lt;br /&gt;• Finish: Sterling Silver ∙ 18K Gold &lt;br /&gt;&lt;br /&gt;• Featuring dainty ~9mm Climber Stud Earrings with ~1-2mm CZ Diamond Gemstones | Sold as a pair&lt;br /&gt;&lt;br /&gt;♡ Model showcases a delicate, everyday look featuring: &lt;br /&gt;• Open Diamond Ring: https://etsy.me/3Frvola&lt;br /&gt;• Box Chain Bracelet: https://etsy.me/3FAhwVD&lt;br /&gt;&lt;br /&gt;O T H E R ∙ I N F O R M A T I O N&lt;br /&gt;&lt;br /&gt;• All items are nicely packaged ready to gift in elegant jewelry boxes. &lt;br /&gt;&lt;br /&gt;• Have any questions or need advice on your custom design? Feel free to contact us. We are fast to reply :)&lt;br /&gt;&lt;br /&gt;T U R N ∙ A R O U N D ∙ T I M E&lt;br /&gt;&lt;br /&gt;• This design is ready to ship in 1 - 2 business days. If you have custom made items in your cart, your order will be separated into two shipments (for U.S. orders only). Our turnaround time is about 6 - 9 business days for custom made designs. This can change during peak seasons. Please check our home page for the most current times. &lt;br /&gt;&lt;br /&gt;M O R E ∙ F R O M ∙ U S&lt;br /&gt;https://www.etsy.com/shop/CaitlynMinimalist&lt;br /&gt;IG: @CaitlynMinimalist&lt;br /&gt;&lt;br /&gt;Thank you so much for visiting and hope you enjoy shopping with us ♡&lt;br /&gt;&lt;br /&gt;Kate ♡&lt;br /&gt;&lt;br /&gt;----------------------------------------------&lt;br /&gt;• All images are copyrighted by CaitlynMinimalist. All rights reserved •&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2514,22 +4243,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Threader Earrings Pendulum Sterling Silver Chain Earrings Dangle Minimalist Jewelry  Gift for Her - CHN001 by Revelmy</t>
+          <t>Suspender Earring Minimalist Silver Earring • Modern Geometric Ear Lobe Cuff Earring • 14k Gold Filled Stud Bar Earring Simple Gift - CST027 by Revelmy</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/522407049/threader-earrings-pendulum-sterling?ref=rss</t>
+          <t>https://www.etsy.com/listing/731082669/suspender-earring-minimalist-silver?ref=rss</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:00:25 -0400</t>
+          <t>Mon, 19 May 2025 15:37:27 -0400</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/45d44e/5150515248/il_570xN.5150515248_qlt2.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;24.90 USD&lt;/p&gt;&lt;p class="description"&gt;Pendulum Chain Earrings cast in solid Sterling Silver (925). Inspired by the mystic soul of the Pendulum symbol. Sold in pairs.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver Option &amp;gt; Made of solid 925 Sterling Silver with an oxidized finish&lt;br /&gt;Gold Plated Option &amp;gt; 18K Gold plated over solid 925 Sterling Silver&lt;br /&gt;Hypo-Allergenic materials for sensitive skin&lt;br /&gt;The whole earring measures 3-1/2&amp;quot; (90mm) long&lt;br /&gt;The pendulum charm size is about 3/8&amp;quot; (9mm). &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;►►See Similar Designs here ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/revelmy?ref=listing-shop2-all-items-count&amp;amp;section_id=16171096&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/7a256a/3934547255/il_570xN.3934547255_6bzy.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;21.90 USD&lt;/p&gt;&lt;p class="description"&gt;Minimalist Ear Suspender Stud Earring. Sold by the piece or pairs. Round Bar Earrings Design, Handmade in solid Sterling Silver or 14K Gold Filled.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver 925 &amp;gt; Made of solid 925 Sterling Silver. Includes a Barrel Earring Back&lt;br /&gt;14K Yellow Gold &amp;gt; 14K Yellow Gold Filled over solid 925 Sterling Silver. Includes a  Butterfly Earring Back&lt;br /&gt;Earring Inner Length &amp;gt; 20mm, 22mm, and 24mm&lt;br /&gt;Half Round Band Width &amp;gt; 1.3mm (about 3/64&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 0.8mm (20g - International Jewelry Standard)&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy S T U D · E A R R I N G S &amp;gt; https://www.etsy.com/shop/Revelmy?ref=simple-shop-header-name&amp;amp;listing_id=698070485&amp;amp;section_id=17520381&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2541,22 +4270,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Stackable Ring Double Arrow Wire Ring Sterling Silver Adjustable Ring Wrap Ring Boho Jewelry  Gift for Her - FRI008 by Revelmy</t>
+          <t>Spider Web Earring Gothic Jewelry • Cartilage Helix Piercing 20G 18G 16G • Halloween Witchy Silver Jewelry • Goth Punk Tattoo Earring CRT015 by Revelmy</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/242493266/stackable-ring-double-arrow-wire-ring?ref=rss</t>
+          <t>https://www.etsy.com/listing/1610950787/spider-web-earring-gothic-jewelry?ref=rss</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:00:25 -0400</t>
+          <t>Mon, 19 May 2025 15:29:48 -0400</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/ae1426/3404220720/il_570xN.3404220720_hxx7.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;26.90 USD&lt;/p&gt;&lt;p class="description"&gt;Stackable Ring Double Arrow Ring made with Sterling Silver wire. Made with shiny polish finish. It can be adjusted in sizes from 6 to 9&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/64fd57/5552112759/il_570xN.5552112759_7glv.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;26.90 USD&lt;/p&gt;&lt;p class="description"&gt;Gothic Spider Web Silver Helix Earring. This design is made of solid 925 Sterling Silver and 316L Surgical Steel. It is finished with an oxidized look and 24K gold plating. Sold by the piece.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S&lt;br /&gt;Frontal design metal &amp;gt; Solid 925 Sterling silver&lt;br /&gt;Back part metal &amp;gt; 316L Surgical Steel&lt;br /&gt;Surface color &amp;gt; 925 Sterling Silver or 24K Gold plating.&lt;br /&gt;&lt;br /&gt;S I Z E S&lt;br /&gt;Frontal design earring Width &amp;gt; 22mm (about 7/8&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 18G (1.0mm) and 16G (1.2mm)&lt;br /&gt;Post Length &amp;gt; 6mm (about 1/4&amp;quot;) and 8mm (about 5/16&amp;quot;)&lt;br /&gt;Backing Type &amp;gt; Flat Back and Screw-Ball&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy Helix Earrings &amp;gt; https://www.revelmy.etsy.com/?etsrc=sdt&amp;amp;etsrc=sdt§ion_id=26853780&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones inspire our jewelry + love for dreaming of unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025 R E V E L M Y · J E W E L R Y&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2568,22 +4297,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Spider Web Earring Gothic Jewelry • Cartilage Helix Piercing 20G 18G 16G • Halloween Witchy Silver Jewelry • Goth Punk Tattoo Earring CRT015 by Revelmy</t>
+          <t>Suspender Earring Minimalist 14k Gold Filled Earring • Modern Geometric Ear Lobe Cuff Earring • Silver Stud Bar Earring Simple Gift - CST027 by Revelmy</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1610950787/spider-web-earring-gothic-jewelry?ref=rss</t>
+          <t>https://www.etsy.com/listing/1768576584/suspender-earring-minimalist-14k-gold?ref=rss</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 18:00:24 -0400</t>
+          <t>Mon, 19 May 2025 14:31:48 -0400</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/64fd57/5552112759/il_570xN.5552112759_7glv.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;25.90 USD&lt;/p&gt;&lt;p class="description"&gt;Gothic Spider Web Silver Helix Earring. This design is made of solid 925 Sterling Silver and 316L Surgical Steel. It is finished with an oxidized look and 24K gold plating. Sold by the piece.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S&lt;br /&gt;Frontal design metal &amp;gt; Solid 925 Sterling silver&lt;br /&gt;Back part metal &amp;gt; 316L Surgical Steel&lt;br /&gt;Surface color &amp;gt; 925 Sterling Silver or 24K Gold plating.&lt;br /&gt;&lt;br /&gt;S I Z E S&lt;br /&gt;Frontal design earring Width &amp;gt; 22mm (about 7/8&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 18G (1.0mm) and 16G (1.2mm)&lt;br /&gt;Post Length &amp;gt; 6mm (about 1/4&amp;quot;) and 8mm (about 5/16&amp;quot;)&lt;br /&gt;Backing Type &amp;gt; Flat Back and Screw-Ball&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy Helix Earrings &amp;gt; https://www.revelmy.etsy.com/?etsrc=sdt&amp;amp;etsrc=sdt§ion_id=26853780&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones inspire our jewelry + love for dreaming of unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025 R E V E L M Y · J E W E L R Y&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/55440f/6217491390/il_570xN.6217491390_7f85.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;21.90 USD&lt;/p&gt;&lt;p class="description"&gt;Minimalist Ear Suspender Stud Earring. Sold by the piece or pairs. Round Bar Earrings Designs, Handmade in solid 14K Gold Filled or Sterling Silver.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver 925 &amp;gt; Made of solid 925 Sterling Silver. Includes a Barrel Earring Back&lt;br /&gt;14K Yellow Gold &amp;gt; 14K Yellow Gold Filled over solid 925 Sterling Silver. Includes a  Butterfly Earring Back&lt;br /&gt;Earring Inner Length &amp;gt; 20mm, 22mm, and 24mm&lt;br /&gt;Half Round Band Width &amp;gt; 1.3mm (about 3/64&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 0.8mm (20g - International Jewelry Standard)&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy S T U D · E A R R I N G S &amp;gt; https://www.etsy.com/shop/Revelmy?ref=simple-shop-header-name&amp;amp;listing_id=698070485&amp;amp;section_id=17520381&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, the warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025 REVELMY JEWELRY&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2595,22 +4324,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sterling Silver Ear Cuff Earrings Antler Deer Earpin Boho Ear Crawler Wrap Earring Bohemian 925 Jewelry Gift Best Christmas Gift - FES006 by Revelmy</t>
+          <t>Cartilage Earring Crescent Moon Helix Earring 20G 18G 16G Sterling Silver Minimalist Stud Piercing Dainty Jewelry Ear Cuff Earring - CRT001 by Revelmy</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/232459920/sterling-silver-ear-cuff-earrings-antler?ref=rss</t>
+          <t>https://www.etsy.com/listing/617910425/cartilage-earring-crescent-moon-helix?ref=rss</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:52:27 -0400</t>
+          <t>Mon, 19 May 2025 14:24:25 -0400</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/582158/3887152930/il_570xN.3887152930_al61.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;22.90 USD&lt;/p&gt;&lt;p class="description"&gt;Antler Deer Horns Ear Cuff cast in solid Sterling Silver. The earring has been lovely carved inspired by wild deer style.  The Earring measures 7/8&amp;quot; (22mm) long. This design is available in two styles: Oxidized Sterling Silver and shiny Yellow Gold plated.&lt;br /&gt;&lt;br /&gt;►►►  See Similar Designs here  ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/revelmy?section_id=16502094&amp;amp;ref=shopsection_leftnav_3&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/aa4bbe/1517750064/il_570xN.1517750064_c1cd.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;19.90 USD&lt;/p&gt;&lt;p class="description"&gt;Crescent Moon Cartilage Earring. It is finished with a high-polish shine. Sold by the piece.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S &lt;br /&gt;Frontal design base metal &amp;gt; Solid 925 Sterling silver&lt;br /&gt;Back part base metal &amp;gt; 316L Surgical Steel &lt;br /&gt;Surface color &amp;gt; 925 Sterling Silver or 24K Gold plating.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S I Z E S&lt;br /&gt;Frontal design earring Width &amp;gt; 22mm (about 7/8&amp;quot;)&lt;br /&gt;&lt;br /&gt;Screw Option&lt;br /&gt;Post Thickness &amp;gt; 18G (1.0mm) and 16G (1.2mm)&lt;br /&gt;Post Length &amp;gt; 6mm (about 1/4&amp;quot;) and 8mm (about 5/16&amp;quot;)&lt;br /&gt;Backing Type &amp;gt; Flat Back and Screw-Ball&lt;br /&gt;&lt;br /&gt;Push-back Barrel Option&lt;br /&gt;Sterling Silver Option &amp;gt; Made of solid 925 Sterling Silver&lt;br /&gt;Gold Plated Option &amp;gt; 18K Gold plated over solid 925 Sterling Silver&lt;br /&gt;Post Thickness &amp;gt; 20G (0.8mm)&lt;br /&gt;Post Length &amp;gt; 3/8 inch (9mm)&lt;br /&gt;Useful Gap &amp;gt; 4-5mm&lt;br /&gt;Backing Type &amp;gt; Push-back Barrel&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy E A R · C U F F · E A R R I N G S &amp;gt; https://www.etsy.com/shop/revelmy?ref=listing-shop-header-item-count&amp;amp;section_id=16502094&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, the warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025 R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;EUIPO - Design Registration: &lt;br /&gt;https://euipo.europa.eu/eSearch/#details/designs/015066336-0002&lt;br /&gt;&lt;br /&gt;Photography Copyright: &lt;br /&gt;https://www.safecreative.org/work/2310245672480-jn-crt-001-sss-model-2v2&lt;br /&gt;https://www.safecreative.org/work/2408099069751-jncrt001sssfbk_316l_v1_revelmy_9_aug_2024&lt;br /&gt;https://www.safecreative.org/work/2310245672473-jn-crt-001-sss-model-ver3&lt;br /&gt;https://www.safecreative.org/work/2408099069744-jncrt001sssfbk_316l_v2_revelmy_9_aug_2024&lt;br /&gt;https://www.safecreative.org/work/2401256760461-jnp-crt-001-ygs-scr_0015_29-06-23_2_revelmy&lt;br /&gt;https://www.safecreative.org/work/2210242486847-juli_subject_oct2200018-1_weet&lt;br /&gt;https://www.safecreative.org/work/1908271782009-jnp-crt-001-frt-sss&lt;br /&gt;https://www.safecreative.org/work/1908271781989-jnp-crt-001-frt-ygs&lt;br /&gt;https://www.safecreative.org/work/1908271782016-jnp-crt-001-frt-rgs&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2632,7 +4361,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:41:47 -0400</t>
+          <t>Mon, 19 May 2025 13:52:30 -0400</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2649,22 +4378,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Fire Opal Cartilage Earring • Flat Back Stud Earring • Sterling Silver 16G Internally Threaded Labret Stud • Opal Piercing Jewelry - CRT011 by Revelmy</t>
+          <t>Clicker Nose Ring • Octopus Tentacle Septum Ring • Hinged Hoop • Silver Clicker Body Jewelry • Cute Unique Septum • 14g 16g Clicker - BSE035 by Revelmy</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1509560329/fire-opal-cartilage-earring-flat-back?ref=rss</t>
+          <t>https://www.etsy.com/listing/1512001033/clicker-nose-ring-octopus-tentacle?ref=rss</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:41:46 -0400</t>
+          <t>Mon, 19 May 2025 12:41:17 -0400</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/0806cd/5047431666/il_570xN.5047431666_rw8x.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;17.90 USD&lt;/p&gt;&lt;p class="description"&gt;Fire Opal Cartilage Earring made of 925 Sterling Silver. Dainty minimal Jewelry for everyday use. This earring combines White &amp; Black tones of shiny polish and hand-burnished oxidized Sterling Silver. SOLD by PIECE (1 Earring).&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver Option &amp;gt; Made of solid 925 Sterling Silver&lt;br /&gt;Gold Plated Option &amp;gt; 18K Gold plated over solid 925 Sterling Silver&lt;br /&gt;Disc diameter &amp;gt; 4.5mm (~1/5&amp;quot;)&lt;br /&gt;Opal Cabochon Diameter &amp;gt; 1.5mm&lt;br /&gt;Bar Length &amp;gt; 6mm (~1/4 inch)&lt;br /&gt;Gauge / Thickness &amp;gt; 16ga (1.2mm)&lt;br /&gt;Backing Type &amp;gt; Threaded screw &amp; flat back&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;►►►  See Similar Designs here  ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/Revelmy?ref=seller-platform-mcnav&amp;amp;section_id=26853780&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, the warmth of Gold &amp; vibrant Gemstones inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/535b66/5086636469/il_570xN.5086636469_egsr.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;34.90 USD&lt;/p&gt;&lt;p class="description"&gt;Clicker septum ring with Octopus Tentacle design. Modern Jewelry with unique style.  Sold by the piece.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver Option &amp;gt; Made of solid 925 Sterling Silver with an oxidized finish&lt;br /&gt;Hypo-Allergenic material for sensitive skin&lt;br /&gt;Septum Thickness Size &amp;gt; 16g (1.3mm) and 14g (1.6mm) &lt;br /&gt;Septum Diameter (hole inside ) &amp;gt; 9mm (about 3/8&amp;quot;)&lt;br /&gt;Septum Outside Size (Bottom to Top) &amp;gt; 13.5mm (about 9/16&amp;quot;)&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;Matching Designs &amp;gt; https://www.etsy.com/shop/revelmy?ref=seller-platform-mcnav&amp;amp;search_query=octopus&lt;br /&gt;All Revelmy S E P T U M · R I N G S &amp;gt; https://www.etsy.com/shop/revelmy?section_id=17366149&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, the warmth of Gold &amp; vibrant Gemstones inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S &amp;gt; https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;W H O L E S A L E &amp;gt; Email us at info@revelmy.com&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2676,22 +4405,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Silver Ear Climber Minimalist Earrings Crescent Moon Sterling Shine Ear Cuff Earrings Modern Jewelry Gift 14K Ear Wrap - FES007 by Revelmy</t>
+          <t>Line Stud Earrings • Square Bar Stud Earrings • Minimalist Bar Stud Earrings • Silver Small Earrings • Everyday Jewelry Tiny Earring CST012 by Revelmy</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/228277382/silver-ear-climber-minimalist-earrings?ref=rss</t>
+          <t>https://www.etsy.com/listing/1782799277/line-stud-earrings-square-bar-stud?ref=rss</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:34:15 -0400</t>
+          <t>Mon, 19 May 2025 12:05:32 -0400</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/57af18/5404826134/il_570xN.5404826134_2adi.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;23.90 USD&lt;/p&gt;&lt;p class="description"&gt;Moon Shine Ear Climber cast in solid Sterling Silver (925). The earring has been lovely carved inspired by moon shapes spirit. The Earring measures 1&amp;quot; (25mm) long. &lt;br /&gt;This design is available in four styles: Shiny Sterling Silver, Yellow Gold plated, Rose Gold plated and, Matte Sterling Silver&lt;br /&gt;&lt;br /&gt;►►►  See Similar Designs here  ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/revelmy?section_id=16502094&amp;amp;ref=shopsection_leftnav_3&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/341482/6217425118/il_570xN.6217425118_hag7.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;9.90 USD&lt;/p&gt;&lt;p class="description"&gt;Small Bar Stud Earrings. Dainty Minimal Jewelry for Everyday Use. This earring combines White &amp; Black tones of shiny polish and hand-burnished oxidized Sterling Silver. SOLD as PIECE (1 Earring), in PAIRS (2 Earrings), or as a SET of 3 PCS. Make your combination. Our model is wearing Small and Medium earrings in the First Picture.&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Siler Optiopn &amp;gt; Solid 925 Sterling Silver&lt;br /&gt;Gold Option &amp;gt; Solid 925 Sterling Silver with 24K Gold plating&lt;br /&gt;&lt;br /&gt;Small Bar Earring Length &amp;gt; 1/5&amp;quot; (5mm) &lt;br /&gt;Medium Bar Earring Length &amp;gt; 3/8&amp;quot; (8.5mm) &lt;br /&gt;Large Bar Earring Length &amp;gt; 1/2&amp;quot; (12mm)&lt;br /&gt;Post Length &amp;gt; 3/8 inch (10mm)&lt;br /&gt;Post Thickness &amp;gt; 20ga (0.8mm)&lt;br /&gt;Backing Type &amp;gt; Silver-Rubber barrel&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;►►►  See Similar Designs here  ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/revelmy?section_id=17520381&amp;amp;ref=shopsection_leftnav_6&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2703,22 +4432,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cartilage Earring Crescent Moon Helix Earring 20G 18G 16G Sterling Silver Minimalist Stud Piercing Dainty Jewelry Ear Cuff Earring - CRT001 by Revelmy</t>
+          <t>Boho Helix Earring • Geometric Mandala Lotus Flower Hidden Helix • Piercing 18G 16G • Cartilage Bohemian Silver Spiritual Jewelry •  CRT023 by Revelmy</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/617910425/cartilage-earring-crescent-moon-helix?ref=rss</t>
+          <t>https://www.etsy.com/listing/4307573718/boho-helix-earring-geometric-mandala?ref=rss</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 17:32:35 -0400</t>
+          <t>Mon, 19 May 2025 10:19:37 -0400</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/aa4bbe/1517750064/il_570xN.1517750064_c1cd.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;19.90 USD&lt;/p&gt;&lt;p class="description"&gt;Crescent Moon Cartilage Earring. It is finished with a high-polish shine. Sold by the piece.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S &lt;br /&gt;Frontal design base metal &amp;gt; Solid 925 Sterling silver&lt;br /&gt;Back part base metal &amp;gt; 316L Surgical Steel &lt;br /&gt;Surface color &amp;gt; 925 Sterling Silver or 24K Gold plating.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S I Z E S&lt;br /&gt;Frontal design earring Width &amp;gt; 22mm (about 7/8&amp;quot;)&lt;br /&gt;&lt;br /&gt;Screw Option&lt;br /&gt;Post Thickness &amp;gt; 18G (1.0mm) and 16G (1.2mm)&lt;br /&gt;Post Length &amp;gt; 6mm (about 1/4&amp;quot;) and 8mm (about 5/16&amp;quot;)&lt;br /&gt;Backing Type &amp;gt; Flat Back and Screw-Ball&lt;br /&gt;&lt;br /&gt;Push-back Barrel Option&lt;br /&gt;Sterling Silver Option &amp;gt; Made of solid 925 Sterling Silver&lt;br /&gt;Gold Plated Option &amp;gt; 18K Gold plated over solid 925 Sterling Silver&lt;br /&gt;Post Thickness &amp;gt; 20G (0.8mm)&lt;br /&gt;Post Length &amp;gt; 3/8 inch (9mm)&lt;br /&gt;Useful Gap &amp;gt; 4-5mm&lt;br /&gt;Backing Type &amp;gt; Push-back Barrel&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy E A R · C U F F · E A R R I N G S &amp;gt; https://www.etsy.com/shop/revelmy?ref=listing-shop-header-item-count&amp;amp;section_id=16502094&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, the warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025 R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;EUIPO - Design Registration: &lt;br /&gt;https://euipo.europa.eu/eSearch/#details/designs/015066336-0002&lt;br /&gt;&lt;br /&gt;Photography Copyright: &lt;br /&gt;https://www.safecreative.org/work/2310245672480-jn-crt-001-sss-model-2v2&lt;br /&gt;https://www.safecreative.org/work/2408099069751-jncrt001sssfbk_316l_v1_revelmy_9_aug_2024&lt;br /&gt;https://www.safecreative.org/work/2310245672473-jn-crt-001-sss-model-ver3&lt;br /&gt;https://www.safecreative.org/work/2408099069744-jncrt001sssfbk_316l_v2_revelmy_9_aug_2024&lt;br /&gt;https://www.safecreative.org/work/2401256760461-jnp-crt-001-ygs-scr_0015_29-06-23_2_revelmy&lt;br /&gt;https://www.safecreative.org/work/2210242486847-juli_subject_oct2200018-1_weet&lt;br /&gt;https://www.safecreative.org/work/1908271782009-jnp-crt-001-frt-sss&lt;br /&gt;https://www.safecreative.org/work/1908271781989-jnp-crt-001-frt-ygs&lt;br /&gt;https://www.safecreative.org/work/1908271782016-jnp-crt-001-frt-rgs&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/11fa7b/6872982408/il_570xN.6872982408_s022.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;27.90 USD&lt;/p&gt;&lt;p class="description"&gt;Lotus Flower Hidden Helix Earring. This design is made of solid 925 Sterling Silver and 316L Surgical Steel. It is finished with an oxidized look and 24K gold plating. Sold by the piece.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S&lt;br /&gt;Frontal design metal &amp;gt; Solid 925 Sterling silver&lt;br /&gt;Back part metal &amp;gt; 316L Surgical Steel&lt;br /&gt;Surface color &amp;gt; 925 Sterling Silver or 24K Gold plating.&lt;br /&gt;&lt;br /&gt;S I Z E S&lt;br /&gt;Frontal design earring Width &amp;gt; 22mm (about 7/8&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 18G (1.0mm) and 16G (1.2mm)&lt;br /&gt;Post Length &amp;gt; 6mm (about 1/4&amp;quot;) and 8mm (about 5/16&amp;quot;)&lt;br /&gt;Backing Type &amp;gt; Flat Back and Screw-Ball&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy Helix Earrings &amp;gt; https://www.revelmy.etsy.com/?etsrc=sdt&amp;amp;etsrc=sdt§ion_id=26853780&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at checkout. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones inspire our jewelry + love for dreaming of unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025 R E V E L M Y · J E W E L R Y&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2730,22 +4459,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Wide Suspender Earring CZ • Gold Lobe Cuff Earrings • Thick Modern Earring • 14k Gold &amp; Silver Ear Suspender Earring • Bar Earring - CST033 by Revelmy</t>
+          <t>Tiny Stud Earrings Set Sterling Silver Geometric Stud Earrings Dainty Studs Everyday Jewelry Triangle Circle Bar Sterling Silver  - CST100 by Revelmy</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/1266175912/wide-suspender-earring-cz-gold-lobe-cuff?ref=rss</t>
+          <t>https://www.etsy.com/listing/628536573/tiny-stud-earrings-set-sterling-silver?ref=rss</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 14:58:49 -0400</t>
+          <t>Mon, 19 May 2025 09:52:37 -0400</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/5ccf9d/4105764637/il_570xN.4105764637_38le.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;28.90 USD&lt;/p&gt;&lt;p class="description"&gt;Wide Ear Suspender Stud Earring with Gold Rutilated Quartz. Sold by the piece. &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver 925 &amp;gt; Made of solid 925 Sterling Silver. &lt;br /&gt;18K Yellow Gold &amp;gt; 18K Yellow Gold over solid 925 Sterling Silver.&lt;br /&gt;Earring Length &amp;gt; 24mm (about 1&amp;quot;)&lt;br /&gt;Half Round Band Width &amp;gt; 4mm (about 5/32&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 0.8mm (20g - International Jewelry Standard)&lt;br /&gt;Backing Type &amp;gt; Silver-Rubber barrel&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy S T U D · E A R R I N G S &amp;gt; https://www.etsy.com/shop/Revelmy?ref=simple-shop-header-name&amp;amp;listing_id=698070485&amp;amp;section_id=17520381&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2022  R E V E L M Y · J E W E L R Y&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/7579af/5198799095/il_570xN.5198799095_q3v4.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;19.90 USD&lt;/p&gt;&lt;p class="description"&gt;Minimalist Geometrical Earrings Set. Asymmetrical Earrings, Small Dainty designs, your Everyday Jewelry. Stud Earrings: Triangle Dot Square Bar made in Sterling Silver. This earring combines shiny polish and hand-burnishedoxidized finish. &lt;br /&gt;&lt;br /&gt;Choose your style and make persona earrings set.&lt;br /&gt;&lt;br /&gt;Oval earring measures 5/16&amp;quot; (7.5mm) long&lt;br /&gt;Rectangle earring measures 3/16&amp;quot; (4.5mm) long&lt;br /&gt;Circle earring measures  5/32&amp;quot; (4mm) diameter &lt;br /&gt;Triangle earring measures 3/16&amp;quot; (4.5mm) on each side&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;►►►  See Similar Designs here  ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/revelmy?section_id=17520381&amp;amp;ref=shopsection_leftnav_6&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
         </is>
       </c>
     </row>
@@ -2757,22 +4486,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Suspender Earring Minimalist Silver Earring • Modern Geometric Ear Lobe Cuff Earring • 14k Gold Filled Stud Bar Earring Simple Gift - CST027 by Revelmy</t>
+          <t>Sterling Silver Ear Jacket Earrings Sunshine Ear Cuff Earrings Modern Jewelry  Gift for Her - JKT002 by Revelmy</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/listing/731082669/suspender-earring-minimalist-silver?ref=rss</t>
+          <t>https://www.etsy.com/listing/270499405/sterling-silver-ear-jacket-earrings?ref=rss</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Sun, 11 May 2025 14:58:49 -0400</t>
+          <t>Mon, 19 May 2025 09:21:04 -0400</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/7a256a/3934547255/il_570xN.3934547255_6bzy.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;21.90 USD&lt;/p&gt;&lt;p class="description"&gt;Minimalist Ear Suspender Stud Earring. Sold by the piece or pairs. Round Bar Earrings Design, Handmade in solid Sterling Silver or 14K Gold Filled.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;M A T E R I A L S ∙ &amp; ∙ S I Z E &lt;br /&gt;&lt;br /&gt;Sterling Silver 925 &amp;gt; Made of solid 925 Sterling Silver. Includes a Barrel Earring Back&lt;br /&gt;14K Yellow Gold &amp;gt; 14K Yellow Gold Filled over solid 925 Sterling Silver. Includes a  Butterfly Earring Back&lt;br /&gt;Earring Inner Length &amp;gt; 20mm, 22mm, and 24mm&lt;br /&gt;Half Round Band Width &amp;gt; 1.3mm (about 3/64&amp;quot;)&lt;br /&gt;Post Thickness &amp;gt; 0.8mm (20g - International Jewelry Standard)&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;S E E · M O R E &lt;br /&gt;&lt;br /&gt;All Revelmy S T U D · E A R R I N G S &amp;gt; https://www.etsy.com/shop/Revelmy?ref=simple-shop-header-name&amp;amp;listing_id=698070485&amp;amp;section_id=17520381&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
+          <t>&lt;p class="image"&gt;&lt;img border="0" height="429" src="https://i.etsystatic.com/10128979/r/il/4064d6/4188574965/il_570xN.4188574965_kt85.jpg" width="570" /&gt;&lt;/p&gt;&lt;p class="price"&gt;19.90 USD&lt;/p&gt;&lt;p class="description"&gt;Sunshine ear jacket earrings cast in solid Sterling Silver 925, finish with black oxide and hand shiny polish. The Earring measures 11/16&amp;quot; (17mm) long. Triangle stud earrings can also be worn separately. &lt;br /&gt;&lt;br /&gt;►►►  See Similar Designs here  ◄◄◄&lt;br /&gt;https://www.etsy.com/shop/revelmy?section_id=17731069&amp;amp;ref=shopsection_leftnav_8&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;L O V E · I T · &amp; · B U Y · I T&lt;br /&gt;&lt;br /&gt;♥ Want it now? Choose your option &amp;gt;&amp;gt; Choose the Qty and &amp;gt;&amp;gt; Click the green &amp;quot;Add to cart&amp;quot; button.&lt;br /&gt;♥ Love it and want to buy it later? Click on the heart to your right that says &amp;quot;Add item to favorites.&amp;quot;&lt;br /&gt;Back to the S H O P: https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P A C K I N G · &amp; · G I F T · W R A P P I N G&lt;br /&gt;&lt;br /&gt;All our pieces are packed in Jewelry Boxes. It will make the perfect moment for yourself or the ones you Love! If certain pieces are intended as gifts, please leave us a note or mark your order as a Gift at check out. No receipt or invoice will be included with your jewelry.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;F O L L O W · U S · O N&lt;br /&gt;&lt;br /&gt;Instagram - https://www.instagram.com/revelmy/&lt;br /&gt;Facebook - https://www.facebook.com/revelmy/&lt;br /&gt;Pinterest - https://www.pinterest.es/Revelmy/&lt;br /&gt;Our Store - https://www.revelmy.com/&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;A B O U T ∙ R E V E L M Y · J E W E L R Y&lt;br /&gt;&lt;br /&gt;Revelmy Jewelry is born from the spirit of natural designs: the light of Silver, warmth of Gold &amp; vibrant Gemstones, inspire our jewelry + love for dreaming unique art &amp;gt; &amp;gt; &amp;gt; https://www.etsy.com/shop/Revelmy&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;P O L I C I E S: https://www.etsy.com/shop/Revelmy#policies&lt;br /&gt;&lt;br /&gt;Designs and Photos protected by Copyright © 2025  REVELMY JEWELRY&lt;/p&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>